<commit_message>
edited the histo fields
</commit_message>
<xml_diff>
--- a/EMX_1.xlsx
+++ b/EMX_1.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
   <si>
     <t>Mouse ID</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>Slices per plate               (or list of numbers for each plate)</t>
+  </si>
+  <si>
+    <t>6,4</t>
   </si>
 </sst>
 </file>
@@ -859,6 +862,78 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -876,78 +951,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1442,16 +1445,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="39" customHeight="1" thickTop="1">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="64" t="s">
+      <c r="B1" s="53"/>
+      <c r="C1" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
       <c r="G1" s="29" t="s">
         <v>31</v>
       </c>
@@ -1460,56 +1463,56 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="39" customHeight="1">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="51" t="s">
+      <c r="B2" s="55"/>
+      <c r="C2" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
       <c r="G2" s="30" t="s">
         <v>31</v>
       </c>
       <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:8" ht="39" customHeight="1">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="61"/>
-      <c r="C3" s="50" t="s">
+      <c r="B3" s="55"/>
+      <c r="C3" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="53"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="47"/>
     </row>
     <row r="4" spans="1:8" ht="102" customHeight="1" thickBot="1">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="63"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="57"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="51"/>
     </row>
     <row r="5" spans="1:8" ht="26" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A5" s="49"/>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
     </row>
     <row r="6" spans="1:8" ht="39" customHeight="1" thickTop="1">
       <c r="A6" s="9" t="s">
@@ -1527,11 +1530,11 @@
       <c r="E6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="46" t="s">
+      <c r="F6" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="47"/>
-      <c r="H6" s="48"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="39"/>
     </row>
     <row r="7" spans="1:8" ht="39" customHeight="1">
       <c r="A7" s="3">
@@ -1543,11 +1546,11 @@
       <c r="C7" s="4"/>
       <c r="D7" s="5"/>
       <c r="E7" s="26"/>
-      <c r="F7" s="43" t="s">
+      <c r="F7" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="G7" s="44"/>
-      <c r="H7" s="45"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="42"/>
     </row>
     <row r="8" spans="1:8" ht="39" customHeight="1">
       <c r="A8" s="3">
@@ -1559,11 +1562,11 @@
       <c r="C8" s="4"/>
       <c r="D8" s="5"/>
       <c r="E8" s="26"/>
-      <c r="F8" s="43" t="s">
+      <c r="F8" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="G8" s="44"/>
-      <c r="H8" s="45"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="42"/>
     </row>
     <row r="9" spans="1:8" ht="39" customHeight="1">
       <c r="A9" s="3">
@@ -1575,11 +1578,11 @@
       <c r="C9" s="4"/>
       <c r="D9" s="5"/>
       <c r="E9" s="26"/>
-      <c r="F9" s="43" t="s">
+      <c r="F9" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="G9" s="44"/>
-      <c r="H9" s="45"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="42"/>
     </row>
     <row r="10" spans="1:8" ht="39" customHeight="1">
       <c r="A10" s="3">
@@ -1591,11 +1594,11 @@
       <c r="C10" s="4"/>
       <c r="D10" s="5"/>
       <c r="E10" s="26"/>
-      <c r="F10" s="43" t="s">
+      <c r="F10" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="G10" s="44"/>
-      <c r="H10" s="45"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="42"/>
     </row>
     <row r="11" spans="1:8" ht="39" customHeight="1">
       <c r="A11" s="3">
@@ -1607,11 +1610,11 @@
       <c r="C11" s="4"/>
       <c r="D11" s="5"/>
       <c r="E11" s="26"/>
-      <c r="F11" s="43" t="s">
+      <c r="F11" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="G11" s="44"/>
-      <c r="H11" s="45"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="42"/>
     </row>
     <row r="12" spans="1:8" ht="39" customHeight="1">
       <c r="A12" s="3">
@@ -1623,11 +1626,11 @@
       <c r="C12" s="4"/>
       <c r="D12" s="5"/>
       <c r="E12" s="26"/>
-      <c r="F12" s="43" t="s">
+      <c r="F12" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="G12" s="44"/>
-      <c r="H12" s="45"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="42"/>
     </row>
     <row r="13" spans="1:8" ht="39" customHeight="1">
       <c r="A13" s="3">
@@ -1639,11 +1642,11 @@
       <c r="C13" s="4"/>
       <c r="D13" s="5"/>
       <c r="E13" s="26"/>
-      <c r="F13" s="43" t="s">
+      <c r="F13" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="44"/>
-      <c r="H13" s="45"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="42"/>
     </row>
     <row r="14" spans="1:8" ht="39" customHeight="1">
       <c r="A14" s="3"/>
@@ -1651,9 +1654,9 @@
       <c r="C14" s="4"/>
       <c r="D14" s="5"/>
       <c r="E14" s="26"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="45"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="42"/>
     </row>
     <row r="15" spans="1:8" ht="39" customHeight="1">
       <c r="A15" s="3"/>
@@ -1661,9 +1664,9 @@
       <c r="C15" s="4"/>
       <c r="D15" s="5"/>
       <c r="E15" s="26"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="45"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="42"/>
     </row>
     <row r="16" spans="1:8" ht="39" customHeight="1">
       <c r="A16" s="3"/>
@@ -1671,9 +1674,9 @@
       <c r="C16" s="4"/>
       <c r="D16" s="5"/>
       <c r="E16" s="26"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="44"/>
-      <c r="H16" s="45"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="42"/>
     </row>
     <row r="17" spans="1:8" ht="39" customHeight="1">
       <c r="A17" s="3"/>
@@ -1681,9 +1684,9 @@
       <c r="C17" s="4"/>
       <c r="D17" s="5"/>
       <c r="E17" s="26"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="45"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="42"/>
     </row>
     <row r="18" spans="1:8" ht="39" customHeight="1">
       <c r="A18" s="3"/>
@@ -1691,9 +1694,9 @@
       <c r="C18" s="4"/>
       <c r="D18" s="5"/>
       <c r="E18" s="26"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="44"/>
-      <c r="H18" s="45"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="42"/>
     </row>
     <row r="19" spans="1:8" ht="39" customHeight="1">
       <c r="A19" s="3"/>
@@ -1701,9 +1704,9 @@
       <c r="C19" s="4"/>
       <c r="D19" s="5"/>
       <c r="E19" s="26"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="44"/>
-      <c r="H19" s="45"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="42"/>
     </row>
     <row r="20" spans="1:8" ht="39" customHeight="1">
       <c r="A20" s="3"/>
@@ -1711,9 +1714,9 @@
       <c r="C20" s="4"/>
       <c r="D20" s="5"/>
       <c r="E20" s="26"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="44"/>
-      <c r="H20" s="45"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="42"/>
     </row>
     <row r="21" spans="1:8" ht="39" customHeight="1">
       <c r="A21" s="3"/>
@@ -1721,9 +1724,9 @@
       <c r="C21" s="4"/>
       <c r="D21" s="5"/>
       <c r="E21" s="26"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="44"/>
-      <c r="H21" s="45"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="42"/>
     </row>
     <row r="22" spans="1:8" ht="39" customHeight="1">
       <c r="A22" s="3"/>
@@ -1731,9 +1734,9 @@
       <c r="C22" s="4"/>
       <c r="D22" s="5"/>
       <c r="E22" s="26"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="44"/>
-      <c r="H22" s="45"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="42"/>
     </row>
     <row r="23" spans="1:8" ht="39" customHeight="1">
       <c r="A23" s="3"/>
@@ -1741,9 +1744,9 @@
       <c r="C23" s="4"/>
       <c r="D23" s="5"/>
       <c r="E23" s="26"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="44"/>
-      <c r="H23" s="45"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="42"/>
     </row>
     <row r="24" spans="1:8" ht="39" customHeight="1">
       <c r="A24" s="3"/>
@@ -1751,9 +1754,9 @@
       <c r="C24" s="4"/>
       <c r="D24" s="5"/>
       <c r="E24" s="26"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="44"/>
-      <c r="H24" s="45"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="42"/>
     </row>
     <row r="25" spans="1:8" ht="39" customHeight="1">
       <c r="A25" s="3"/>
@@ -1761,9 +1764,9 @@
       <c r="C25" s="4"/>
       <c r="D25" s="5"/>
       <c r="E25" s="26"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="44"/>
-      <c r="H25" s="45"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="41"/>
+      <c r="H25" s="42"/>
     </row>
     <row r="26" spans="1:8" ht="39" customHeight="1">
       <c r="A26" s="3"/>
@@ -1771,9 +1774,9 @@
       <c r="C26" s="4"/>
       <c r="D26" s="5"/>
       <c r="E26" s="26"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="44"/>
-      <c r="H26" s="45"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="41"/>
+      <c r="H26" s="42"/>
     </row>
     <row r="27" spans="1:8" ht="39" customHeight="1">
       <c r="A27" s="3"/>
@@ -1781,9 +1784,9 @@
       <c r="C27" s="4"/>
       <c r="D27" s="5"/>
       <c r="E27" s="26"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="45"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="42"/>
     </row>
     <row r="28" spans="1:8" ht="39" customHeight="1">
       <c r="A28" s="3"/>
@@ -1791,9 +1794,9 @@
       <c r="C28" s="4"/>
       <c r="D28" s="5"/>
       <c r="E28" s="26"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="44"/>
-      <c r="H28" s="45"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="41"/>
+      <c r="H28" s="42"/>
     </row>
     <row r="29" spans="1:8" ht="39" customHeight="1">
       <c r="A29" s="3"/>
@@ -1801,9 +1804,9 @@
       <c r="C29" s="4"/>
       <c r="D29" s="5"/>
       <c r="E29" s="26"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="45"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="41"/>
+      <c r="H29" s="42"/>
     </row>
     <row r="30" spans="1:8" ht="39" customHeight="1">
       <c r="A30" s="3"/>
@@ -1811,9 +1814,9 @@
       <c r="C30" s="4"/>
       <c r="D30" s="5"/>
       <c r="E30" s="26"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="45"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="42"/>
     </row>
     <row r="31" spans="1:8" ht="39" customHeight="1">
       <c r="A31" s="3"/>
@@ -1821,9 +1824,9 @@
       <c r="C31" s="4"/>
       <c r="D31" s="5"/>
       <c r="E31" s="26"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="44"/>
-      <c r="H31" s="45"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="42"/>
     </row>
     <row r="32" spans="1:8" ht="39" customHeight="1">
       <c r="A32" s="3"/>
@@ -1831,9 +1834,9 @@
       <c r="C32" s="4"/>
       <c r="D32" s="5"/>
       <c r="E32" s="26"/>
-      <c r="F32" s="43"/>
-      <c r="G32" s="44"/>
-      <c r="H32" s="45"/>
+      <c r="F32" s="40"/>
+      <c r="G32" s="41"/>
+      <c r="H32" s="42"/>
     </row>
     <row r="33" spans="1:8" ht="39" customHeight="1">
       <c r="A33" s="3"/>
@@ -1841,9 +1844,9 @@
       <c r="C33" s="4"/>
       <c r="D33" s="5"/>
       <c r="E33" s="26"/>
-      <c r="F33" s="43"/>
-      <c r="G33" s="44"/>
-      <c r="H33" s="45"/>
+      <c r="F33" s="40"/>
+      <c r="G33" s="41"/>
+      <c r="H33" s="42"/>
     </row>
     <row r="34" spans="1:8" ht="39" customHeight="1">
       <c r="A34" s="3"/>
@@ -1851,9 +1854,9 @@
       <c r="C34" s="4"/>
       <c r="D34" s="5"/>
       <c r="E34" s="26"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="44"/>
-      <c r="H34" s="45"/>
+      <c r="F34" s="40"/>
+      <c r="G34" s="41"/>
+      <c r="H34" s="42"/>
     </row>
     <row r="35" spans="1:8" ht="39" customHeight="1">
       <c r="A35" s="3"/>
@@ -1861,9 +1864,9 @@
       <c r="C35" s="4"/>
       <c r="D35" s="5"/>
       <c r="E35" s="26"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="44"/>
-      <c r="H35" s="45"/>
+      <c r="F35" s="40"/>
+      <c r="G35" s="41"/>
+      <c r="H35" s="42"/>
     </row>
     <row r="36" spans="1:8" ht="39" customHeight="1">
       <c r="A36" s="3"/>
@@ -1871,9 +1874,9 @@
       <c r="C36" s="4"/>
       <c r="D36" s="5"/>
       <c r="E36" s="26"/>
-      <c r="F36" s="43"/>
-      <c r="G36" s="44"/>
-      <c r="H36" s="45"/>
+      <c r="F36" s="40"/>
+      <c r="G36" s="41"/>
+      <c r="H36" s="42"/>
     </row>
     <row r="37" spans="1:8" ht="39" customHeight="1">
       <c r="A37" s="3"/>
@@ -1881,9 +1884,9 @@
       <c r="C37" s="4"/>
       <c r="D37" s="5"/>
       <c r="E37" s="26"/>
-      <c r="F37" s="43"/>
-      <c r="G37" s="44"/>
-      <c r="H37" s="45"/>
+      <c r="F37" s="40"/>
+      <c r="G37" s="41"/>
+      <c r="H37" s="42"/>
     </row>
     <row r="38" spans="1:8" ht="39" customHeight="1">
       <c r="A38" s="3"/>
@@ -1891,9 +1894,9 @@
       <c r="C38" s="4"/>
       <c r="D38" s="5"/>
       <c r="E38" s="26"/>
-      <c r="F38" s="43"/>
-      <c r="G38" s="44"/>
-      <c r="H38" s="45"/>
+      <c r="F38" s="40"/>
+      <c r="G38" s="41"/>
+      <c r="H38" s="42"/>
     </row>
     <row r="39" spans="1:8" ht="39" customHeight="1">
       <c r="A39" s="3"/>
@@ -1901,9 +1904,9 @@
       <c r="C39" s="4"/>
       <c r="D39" s="5"/>
       <c r="E39" s="26"/>
-      <c r="F39" s="43"/>
-      <c r="G39" s="44"/>
-      <c r="H39" s="45"/>
+      <c r="F39" s="40"/>
+      <c r="G39" s="41"/>
+      <c r="H39" s="42"/>
     </row>
     <row r="40" spans="1:8" ht="39" customHeight="1">
       <c r="A40" s="3"/>
@@ -1911,9 +1914,9 @@
       <c r="C40" s="4"/>
       <c r="D40" s="5"/>
       <c r="E40" s="26"/>
-      <c r="F40" s="43"/>
-      <c r="G40" s="44"/>
-      <c r="H40" s="45"/>
+      <c r="F40" s="40"/>
+      <c r="G40" s="41"/>
+      <c r="H40" s="42"/>
     </row>
     <row r="41" spans="1:8" ht="39" customHeight="1">
       <c r="A41" s="3"/>
@@ -1921,9 +1924,9 @@
       <c r="C41" s="4"/>
       <c r="D41" s="5"/>
       <c r="E41" s="26"/>
-      <c r="F41" s="43"/>
-      <c r="G41" s="44"/>
-      <c r="H41" s="45"/>
+      <c r="F41" s="40"/>
+      <c r="G41" s="41"/>
+      <c r="H41" s="42"/>
     </row>
     <row r="42" spans="1:8" ht="39" customHeight="1">
       <c r="A42" s="3"/>
@@ -1931,9 +1934,9 @@
       <c r="C42" s="4"/>
       <c r="D42" s="5"/>
       <c r="E42" s="26"/>
-      <c r="F42" s="43"/>
-      <c r="G42" s="44"/>
-      <c r="H42" s="45"/>
+      <c r="F42" s="40"/>
+      <c r="G42" s="41"/>
+      <c r="H42" s="42"/>
     </row>
     <row r="43" spans="1:8" ht="39" customHeight="1">
       <c r="A43" s="3"/>
@@ -1941,9 +1944,9 @@
       <c r="C43" s="4"/>
       <c r="D43" s="5"/>
       <c r="E43" s="26"/>
-      <c r="F43" s="43"/>
-      <c r="G43" s="44"/>
-      <c r="H43" s="45"/>
+      <c r="F43" s="40"/>
+      <c r="G43" s="41"/>
+      <c r="H43" s="42"/>
     </row>
     <row r="44" spans="1:8" ht="39" customHeight="1">
       <c r="A44" s="3"/>
@@ -1951,9 +1954,9 @@
       <c r="C44" s="4"/>
       <c r="D44" s="5"/>
       <c r="E44" s="26"/>
-      <c r="F44" s="43"/>
-      <c r="G44" s="44"/>
-      <c r="H44" s="45"/>
+      <c r="F44" s="40"/>
+      <c r="G44" s="41"/>
+      <c r="H44" s="42"/>
     </row>
     <row r="45" spans="1:8" ht="39" customHeight="1">
       <c r="A45" s="3"/>
@@ -1961,9 +1964,9 @@
       <c r="C45" s="4"/>
       <c r="D45" s="5"/>
       <c r="E45" s="26"/>
-      <c r="F45" s="43"/>
-      <c r="G45" s="44"/>
-      <c r="H45" s="45"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="41"/>
+      <c r="H45" s="42"/>
     </row>
     <row r="46" spans="1:8" ht="39" customHeight="1">
       <c r="A46" s="3"/>
@@ -1971,9 +1974,9 @@
       <c r="C46" s="4"/>
       <c r="D46" s="5"/>
       <c r="E46" s="26"/>
-      <c r="F46" s="43"/>
-      <c r="G46" s="44"/>
-      <c r="H46" s="45"/>
+      <c r="F46" s="40"/>
+      <c r="G46" s="41"/>
+      <c r="H46" s="42"/>
     </row>
     <row r="47" spans="1:8" ht="39" customHeight="1">
       <c r="A47" s="3"/>
@@ -1981,9 +1984,9 @@
       <c r="C47" s="4"/>
       <c r="D47" s="5"/>
       <c r="E47" s="26"/>
-      <c r="F47" s="43"/>
-      <c r="G47" s="44"/>
-      <c r="H47" s="45"/>
+      <c r="F47" s="40"/>
+      <c r="G47" s="41"/>
+      <c r="H47" s="42"/>
     </row>
     <row r="48" spans="1:8" ht="39" customHeight="1">
       <c r="A48" s="3"/>
@@ -1991,9 +1994,9 @@
       <c r="C48" s="4"/>
       <c r="D48" s="5"/>
       <c r="E48" s="26"/>
-      <c r="F48" s="43"/>
-      <c r="G48" s="44"/>
-      <c r="H48" s="45"/>
+      <c r="F48" s="40"/>
+      <c r="G48" s="41"/>
+      <c r="H48" s="42"/>
     </row>
     <row r="49" spans="1:8" ht="39" customHeight="1">
       <c r="A49" s="3"/>
@@ -2001,9 +2004,9 @@
       <c r="C49" s="4"/>
       <c r="D49" s="5"/>
       <c r="E49" s="26"/>
-      <c r="F49" s="43"/>
-      <c r="G49" s="44"/>
-      <c r="H49" s="45"/>
+      <c r="F49" s="40"/>
+      <c r="G49" s="41"/>
+      <c r="H49" s="42"/>
     </row>
     <row r="50" spans="1:8" ht="39" customHeight="1">
       <c r="A50" s="3"/>
@@ -2011,9 +2014,9 @@
       <c r="C50" s="4"/>
       <c r="D50" s="5"/>
       <c r="E50" s="26"/>
-      <c r="F50" s="43"/>
-      <c r="G50" s="44"/>
-      <c r="H50" s="45"/>
+      <c r="F50" s="40"/>
+      <c r="G50" s="41"/>
+      <c r="H50" s="42"/>
     </row>
     <row r="51" spans="1:8" ht="39" customHeight="1">
       <c r="A51" s="3"/>
@@ -2021,9 +2024,9 @@
       <c r="C51" s="4"/>
       <c r="D51" s="5"/>
       <c r="E51" s="26"/>
-      <c r="F51" s="43"/>
-      <c r="G51" s="44"/>
-      <c r="H51" s="45"/>
+      <c r="F51" s="40"/>
+      <c r="G51" s="41"/>
+      <c r="H51" s="42"/>
     </row>
     <row r="52" spans="1:8" ht="39" customHeight="1">
       <c r="A52" s="3"/>
@@ -2031,9 +2034,9 @@
       <c r="C52" s="4"/>
       <c r="D52" s="5"/>
       <c r="E52" s="26"/>
-      <c r="F52" s="43"/>
-      <c r="G52" s="44"/>
-      <c r="H52" s="45"/>
+      <c r="F52" s="40"/>
+      <c r="G52" s="41"/>
+      <c r="H52" s="42"/>
     </row>
     <row r="53" spans="1:8" ht="39" customHeight="1">
       <c r="A53" s="3"/>
@@ -2041,9 +2044,9 @@
       <c r="C53" s="4"/>
       <c r="D53" s="5"/>
       <c r="E53" s="26"/>
-      <c r="F53" s="43"/>
-      <c r="G53" s="44"/>
-      <c r="H53" s="45"/>
+      <c r="F53" s="40"/>
+      <c r="G53" s="41"/>
+      <c r="H53" s="42"/>
     </row>
     <row r="54" spans="1:8" ht="39" customHeight="1">
       <c r="A54" s="3"/>
@@ -2051,9 +2054,9 @@
       <c r="C54" s="4"/>
       <c r="D54" s="5"/>
       <c r="E54" s="26"/>
-      <c r="F54" s="43"/>
-      <c r="G54" s="44"/>
-      <c r="H54" s="45"/>
+      <c r="F54" s="40"/>
+      <c r="G54" s="41"/>
+      <c r="H54" s="42"/>
     </row>
     <row r="55" spans="1:8" ht="39" customHeight="1">
       <c r="A55" s="3"/>
@@ -2061,9 +2064,9 @@
       <c r="C55" s="4"/>
       <c r="D55" s="5"/>
       <c r="E55" s="26"/>
-      <c r="F55" s="43"/>
-      <c r="G55" s="44"/>
-      <c r="H55" s="45"/>
+      <c r="F55" s="40"/>
+      <c r="G55" s="41"/>
+      <c r="H55" s="42"/>
     </row>
     <row r="56" spans="1:8" ht="39" customHeight="1">
       <c r="A56" s="3"/>
@@ -2071,9 +2074,9 @@
       <c r="C56" s="4"/>
       <c r="D56" s="5"/>
       <c r="E56" s="26"/>
-      <c r="F56" s="43"/>
-      <c r="G56" s="44"/>
-      <c r="H56" s="45"/>
+      <c r="F56" s="40"/>
+      <c r="G56" s="41"/>
+      <c r="H56" s="42"/>
     </row>
     <row r="57" spans="1:8" ht="39" customHeight="1">
       <c r="A57" s="3"/>
@@ -2081,9 +2084,9 @@
       <c r="C57" s="4"/>
       <c r="D57" s="5"/>
       <c r="E57" s="26"/>
-      <c r="F57" s="43"/>
-      <c r="G57" s="44"/>
-      <c r="H57" s="45"/>
+      <c r="F57" s="40"/>
+      <c r="G57" s="41"/>
+      <c r="H57" s="42"/>
     </row>
     <row r="58" spans="1:8" ht="39" customHeight="1">
       <c r="A58" s="3"/>
@@ -2091,9 +2094,9 @@
       <c r="C58" s="4"/>
       <c r="D58" s="5"/>
       <c r="E58" s="26"/>
-      <c r="F58" s="43"/>
-      <c r="G58" s="44"/>
-      <c r="H58" s="45"/>
+      <c r="F58" s="40"/>
+      <c r="G58" s="41"/>
+      <c r="H58" s="42"/>
     </row>
     <row r="59" spans="1:8" ht="39" customHeight="1">
       <c r="A59" s="3"/>
@@ -2101,9 +2104,9 @@
       <c r="C59" s="4"/>
       <c r="D59" s="5"/>
       <c r="E59" s="26"/>
-      <c r="F59" s="43"/>
-      <c r="G59" s="44"/>
-      <c r="H59" s="45"/>
+      <c r="F59" s="40"/>
+      <c r="G59" s="41"/>
+      <c r="H59" s="42"/>
     </row>
     <row r="60" spans="1:8" ht="39" customHeight="1">
       <c r="A60" s="3"/>
@@ -2111,9 +2114,9 @@
       <c r="C60" s="4"/>
       <c r="D60" s="5"/>
       <c r="E60" s="26"/>
-      <c r="F60" s="43"/>
-      <c r="G60" s="44"/>
-      <c r="H60" s="45"/>
+      <c r="F60" s="40"/>
+      <c r="G60" s="41"/>
+      <c r="H60" s="42"/>
     </row>
     <row r="61" spans="1:8" ht="39" customHeight="1">
       <c r="A61" s="3"/>
@@ -2121,9 +2124,9 @@
       <c r="C61" s="4"/>
       <c r="D61" s="5"/>
       <c r="E61" s="26"/>
-      <c r="F61" s="43"/>
-      <c r="G61" s="44"/>
-      <c r="H61" s="45"/>
+      <c r="F61" s="40"/>
+      <c r="G61" s="41"/>
+      <c r="H61" s="42"/>
     </row>
     <row r="62" spans="1:8" ht="39" customHeight="1">
       <c r="A62" s="3"/>
@@ -2131,9 +2134,9 @@
       <c r="C62" s="4"/>
       <c r="D62" s="5"/>
       <c r="E62" s="26"/>
-      <c r="F62" s="43"/>
-      <c r="G62" s="44"/>
-      <c r="H62" s="45"/>
+      <c r="F62" s="40"/>
+      <c r="G62" s="41"/>
+      <c r="H62" s="42"/>
     </row>
     <row r="63" spans="1:8" ht="39" customHeight="1">
       <c r="A63" s="3"/>
@@ -2141,9 +2144,9 @@
       <c r="C63" s="4"/>
       <c r="D63" s="5"/>
       <c r="E63" s="26"/>
-      <c r="F63" s="43"/>
-      <c r="G63" s="44"/>
-      <c r="H63" s="45"/>
+      <c r="F63" s="40"/>
+      <c r="G63" s="41"/>
+      <c r="H63" s="42"/>
     </row>
     <row r="64" spans="1:8" ht="39" customHeight="1">
       <c r="A64" s="3"/>
@@ -2151,9 +2154,9 @@
       <c r="C64" s="4"/>
       <c r="D64" s="5"/>
       <c r="E64" s="26"/>
-      <c r="F64" s="43"/>
-      <c r="G64" s="44"/>
-      <c r="H64" s="45"/>
+      <c r="F64" s="40"/>
+      <c r="G64" s="41"/>
+      <c r="H64" s="42"/>
     </row>
     <row r="65" spans="1:8" ht="39" customHeight="1">
       <c r="A65" s="3"/>
@@ -2161,9 +2164,9 @@
       <c r="C65" s="4"/>
       <c r="D65" s="5"/>
       <c r="E65" s="26"/>
-      <c r="F65" s="43"/>
-      <c r="G65" s="44"/>
-      <c r="H65" s="45"/>
+      <c r="F65" s="40"/>
+      <c r="G65" s="41"/>
+      <c r="H65" s="42"/>
     </row>
     <row r="66" spans="1:8" ht="39" customHeight="1">
       <c r="A66" s="3"/>
@@ -2171,9 +2174,9 @@
       <c r="C66" s="4"/>
       <c r="D66" s="5"/>
       <c r="E66" s="26"/>
-      <c r="F66" s="43"/>
-      <c r="G66" s="44"/>
-      <c r="H66" s="45"/>
+      <c r="F66" s="40"/>
+      <c r="G66" s="41"/>
+      <c r="H66" s="42"/>
     </row>
     <row r="67" spans="1:8" ht="39" customHeight="1">
       <c r="A67" s="3"/>
@@ -2181,9 +2184,9 @@
       <c r="C67" s="4"/>
       <c r="D67" s="5"/>
       <c r="E67" s="26"/>
-      <c r="F67" s="43"/>
-      <c r="G67" s="44"/>
-      <c r="H67" s="45"/>
+      <c r="F67" s="40"/>
+      <c r="G67" s="41"/>
+      <c r="H67" s="42"/>
     </row>
     <row r="68" spans="1:8" ht="39" customHeight="1">
       <c r="A68" s="3"/>
@@ -2191,9 +2194,9 @@
       <c r="C68" s="4"/>
       <c r="D68" s="5"/>
       <c r="E68" s="26"/>
-      <c r="F68" s="43"/>
-      <c r="G68" s="44"/>
-      <c r="H68" s="45"/>
+      <c r="F68" s="40"/>
+      <c r="G68" s="41"/>
+      <c r="H68" s="42"/>
     </row>
     <row r="69" spans="1:8" ht="39" customHeight="1">
       <c r="A69" s="3"/>
@@ -2201,9 +2204,9 @@
       <c r="C69" s="4"/>
       <c r="D69" s="5"/>
       <c r="E69" s="26"/>
-      <c r="F69" s="43"/>
-      <c r="G69" s="44"/>
-      <c r="H69" s="45"/>
+      <c r="F69" s="40"/>
+      <c r="G69" s="41"/>
+      <c r="H69" s="42"/>
     </row>
     <row r="70" spans="1:8" ht="39" customHeight="1">
       <c r="A70" s="3"/>
@@ -2211,9 +2214,9 @@
       <c r="C70" s="4"/>
       <c r="D70" s="5"/>
       <c r="E70" s="26"/>
-      <c r="F70" s="43"/>
-      <c r="G70" s="44"/>
-      <c r="H70" s="45"/>
+      <c r="F70" s="40"/>
+      <c r="G70" s="41"/>
+      <c r="H70" s="42"/>
     </row>
     <row r="71" spans="1:8" ht="39" customHeight="1">
       <c r="A71" s="3"/>
@@ -2221,9 +2224,9 @@
       <c r="C71" s="4"/>
       <c r="D71" s="5"/>
       <c r="E71" s="26"/>
-      <c r="F71" s="43"/>
-      <c r="G71" s="44"/>
-      <c r="H71" s="45"/>
+      <c r="F71" s="40"/>
+      <c r="G71" s="41"/>
+      <c r="H71" s="42"/>
     </row>
     <row r="72" spans="1:8" ht="39" customHeight="1">
       <c r="A72" s="3"/>
@@ -2231,9 +2234,9 @@
       <c r="C72" s="4"/>
       <c r="D72" s="5"/>
       <c r="E72" s="26"/>
-      <c r="F72" s="43"/>
-      <c r="G72" s="44"/>
-      <c r="H72" s="45"/>
+      <c r="F72" s="40"/>
+      <c r="G72" s="41"/>
+      <c r="H72" s="42"/>
     </row>
     <row r="73" spans="1:8" ht="39" customHeight="1">
       <c r="A73" s="3"/>
@@ -2241,9 +2244,9 @@
       <c r="C73" s="4"/>
       <c r="D73" s="5"/>
       <c r="E73" s="26"/>
-      <c r="F73" s="43"/>
-      <c r="G73" s="44"/>
-      <c r="H73" s="45"/>
+      <c r="F73" s="40"/>
+      <c r="G73" s="41"/>
+      <c r="H73" s="42"/>
     </row>
     <row r="74" spans="1:8" ht="39" customHeight="1">
       <c r="A74" s="3"/>
@@ -2251,9 +2254,9 @@
       <c r="C74" s="4"/>
       <c r="D74" s="5"/>
       <c r="E74" s="26"/>
-      <c r="F74" s="43"/>
-      <c r="G74" s="44"/>
-      <c r="H74" s="45"/>
+      <c r="F74" s="40"/>
+      <c r="G74" s="41"/>
+      <c r="H74" s="42"/>
     </row>
     <row r="75" spans="1:8" ht="39" customHeight="1">
       <c r="A75" s="3"/>
@@ -2261,9 +2264,9 @@
       <c r="C75" s="4"/>
       <c r="D75" s="5"/>
       <c r="E75" s="26"/>
-      <c r="F75" s="43"/>
-      <c r="G75" s="44"/>
-      <c r="H75" s="45"/>
+      <c r="F75" s="40"/>
+      <c r="G75" s="41"/>
+      <c r="H75" s="42"/>
     </row>
     <row r="76" spans="1:8" ht="39" customHeight="1">
       <c r="A76" s="3"/>
@@ -2271,9 +2274,9 @@
       <c r="C76" s="4"/>
       <c r="D76" s="5"/>
       <c r="E76" s="26"/>
-      <c r="F76" s="43"/>
-      <c r="G76" s="44"/>
-      <c r="H76" s="45"/>
+      <c r="F76" s="40"/>
+      <c r="G76" s="41"/>
+      <c r="H76" s="42"/>
     </row>
     <row r="77" spans="1:8" ht="39" customHeight="1">
       <c r="A77" s="3"/>
@@ -2281,9 +2284,9 @@
       <c r="C77" s="4"/>
       <c r="D77" s="5"/>
       <c r="E77" s="26"/>
-      <c r="F77" s="43"/>
-      <c r="G77" s="44"/>
-      <c r="H77" s="45"/>
+      <c r="F77" s="40"/>
+      <c r="G77" s="41"/>
+      <c r="H77" s="42"/>
     </row>
     <row r="78" spans="1:8" ht="39" customHeight="1">
       <c r="A78" s="3"/>
@@ -2291,9 +2294,9 @@
       <c r="C78" s="4"/>
       <c r="D78" s="5"/>
       <c r="E78" s="26"/>
-      <c r="F78" s="43"/>
-      <c r="G78" s="44"/>
-      <c r="H78" s="45"/>
+      <c r="F78" s="40"/>
+      <c r="G78" s="41"/>
+      <c r="H78" s="42"/>
     </row>
     <row r="79" spans="1:8" ht="39" customHeight="1">
       <c r="A79" s="3"/>
@@ -2301,9 +2304,9 @@
       <c r="C79" s="4"/>
       <c r="D79" s="5"/>
       <c r="E79" s="26"/>
-      <c r="F79" s="43"/>
-      <c r="G79" s="44"/>
-      <c r="H79" s="45"/>
+      <c r="F79" s="40"/>
+      <c r="G79" s="41"/>
+      <c r="H79" s="42"/>
     </row>
     <row r="80" spans="1:8" ht="39" customHeight="1">
       <c r="A80" s="3"/>
@@ -2311,9 +2314,9 @@
       <c r="C80" s="4"/>
       <c r="D80" s="5"/>
       <c r="E80" s="26"/>
-      <c r="F80" s="43"/>
-      <c r="G80" s="44"/>
-      <c r="H80" s="45"/>
+      <c r="F80" s="40"/>
+      <c r="G80" s="41"/>
+      <c r="H80" s="42"/>
     </row>
     <row r="81" spans="1:8" ht="39" customHeight="1">
       <c r="A81" s="3"/>
@@ -2321,9 +2324,9 @@
       <c r="C81" s="4"/>
       <c r="D81" s="5"/>
       <c r="E81" s="26"/>
-      <c r="F81" s="43"/>
-      <c r="G81" s="44"/>
-      <c r="H81" s="45"/>
+      <c r="F81" s="40"/>
+      <c r="G81" s="41"/>
+      <c r="H81" s="42"/>
     </row>
     <row r="82" spans="1:8" ht="39" customHeight="1">
       <c r="A82" s="3"/>
@@ -2331,9 +2334,9 @@
       <c r="C82" s="4"/>
       <c r="D82" s="5"/>
       <c r="E82" s="26"/>
-      <c r="F82" s="43"/>
-      <c r="G82" s="44"/>
-      <c r="H82" s="45"/>
+      <c r="F82" s="40"/>
+      <c r="G82" s="41"/>
+      <c r="H82" s="42"/>
     </row>
     <row r="83" spans="1:8" ht="39" customHeight="1">
       <c r="A83" s="3"/>
@@ -2341,9 +2344,9 @@
       <c r="C83" s="4"/>
       <c r="D83" s="5"/>
       <c r="E83" s="26"/>
-      <c r="F83" s="43"/>
-      <c r="G83" s="44"/>
-      <c r="H83" s="45"/>
+      <c r="F83" s="40"/>
+      <c r="G83" s="41"/>
+      <c r="H83" s="42"/>
     </row>
     <row r="84" spans="1:8" ht="39" customHeight="1">
       <c r="A84" s="3"/>
@@ -2351,9 +2354,9 @@
       <c r="C84" s="4"/>
       <c r="D84" s="5"/>
       <c r="E84" s="26"/>
-      <c r="F84" s="43"/>
-      <c r="G84" s="44"/>
-      <c r="H84" s="45"/>
+      <c r="F84" s="40"/>
+      <c r="G84" s="41"/>
+      <c r="H84" s="42"/>
     </row>
     <row r="85" spans="1:8" ht="39" customHeight="1">
       <c r="A85" s="3"/>
@@ -2361,9 +2364,9 @@
       <c r="C85" s="4"/>
       <c r="D85" s="5"/>
       <c r="E85" s="26"/>
-      <c r="F85" s="43"/>
-      <c r="G85" s="44"/>
-      <c r="H85" s="45"/>
+      <c r="F85" s="40"/>
+      <c r="G85" s="41"/>
+      <c r="H85" s="42"/>
     </row>
     <row r="86" spans="1:8" ht="39" customHeight="1">
       <c r="A86" s="3"/>
@@ -2371,9 +2374,9 @@
       <c r="C86" s="4"/>
       <c r="D86" s="5"/>
       <c r="E86" s="26"/>
-      <c r="F86" s="43"/>
-      <c r="G86" s="44"/>
-      <c r="H86" s="45"/>
+      <c r="F86" s="40"/>
+      <c r="G86" s="41"/>
+      <c r="H86" s="42"/>
     </row>
     <row r="87" spans="1:8" ht="39" customHeight="1">
       <c r="A87" s="3"/>
@@ -2381,9 +2384,9 @@
       <c r="C87" s="4"/>
       <c r="D87" s="5"/>
       <c r="E87" s="26"/>
-      <c r="F87" s="43"/>
-      <c r="G87" s="44"/>
-      <c r="H87" s="45"/>
+      <c r="F87" s="40"/>
+      <c r="G87" s="41"/>
+      <c r="H87" s="42"/>
     </row>
     <row r="88" spans="1:8" ht="39" customHeight="1">
       <c r="A88" s="3"/>
@@ -2391,9 +2394,9 @@
       <c r="C88" s="4"/>
       <c r="D88" s="5"/>
       <c r="E88" s="26"/>
-      <c r="F88" s="43"/>
-      <c r="G88" s="44"/>
-      <c r="H88" s="45"/>
+      <c r="F88" s="40"/>
+      <c r="G88" s="41"/>
+      <c r="H88" s="42"/>
     </row>
     <row r="89" spans="1:8" ht="39" customHeight="1">
       <c r="A89" s="3"/>
@@ -2401,9 +2404,9 @@
       <c r="C89" s="4"/>
       <c r="D89" s="5"/>
       <c r="E89" s="26"/>
-      <c r="F89" s="43"/>
-      <c r="G89" s="44"/>
-      <c r="H89" s="45"/>
+      <c r="F89" s="40"/>
+      <c r="G89" s="41"/>
+      <c r="H89" s="42"/>
     </row>
     <row r="90" spans="1:8" ht="39" customHeight="1">
       <c r="A90" s="3"/>
@@ -2411,9 +2414,9 @@
       <c r="C90" s="4"/>
       <c r="D90" s="5"/>
       <c r="E90" s="26"/>
-      <c r="F90" s="43"/>
-      <c r="G90" s="44"/>
-      <c r="H90" s="45"/>
+      <c r="F90" s="40"/>
+      <c r="G90" s="41"/>
+      <c r="H90" s="42"/>
     </row>
     <row r="91" spans="1:8" ht="39" customHeight="1">
       <c r="A91" s="3"/>
@@ -2421,9 +2424,9 @@
       <c r="C91" s="4"/>
       <c r="D91" s="5"/>
       <c r="E91" s="26"/>
-      <c r="F91" s="43"/>
-      <c r="G91" s="44"/>
-      <c r="H91" s="45"/>
+      <c r="F91" s="40"/>
+      <c r="G91" s="41"/>
+      <c r="H91" s="42"/>
     </row>
     <row r="92" spans="1:8" ht="39" customHeight="1">
       <c r="A92" s="3"/>
@@ -2431,9 +2434,9 @@
       <c r="C92" s="4"/>
       <c r="D92" s="5"/>
       <c r="E92" s="26"/>
-      <c r="F92" s="43"/>
-      <c r="G92" s="44"/>
-      <c r="H92" s="45"/>
+      <c r="F92" s="40"/>
+      <c r="G92" s="41"/>
+      <c r="H92" s="42"/>
     </row>
     <row r="93" spans="1:8" ht="39" customHeight="1">
       <c r="A93" s="3"/>
@@ -2441,9 +2444,9 @@
       <c r="C93" s="4"/>
       <c r="D93" s="5"/>
       <c r="E93" s="26"/>
-      <c r="F93" s="43"/>
-      <c r="G93" s="44"/>
-      <c r="H93" s="45"/>
+      <c r="F93" s="40"/>
+      <c r="G93" s="41"/>
+      <c r="H93" s="42"/>
     </row>
     <row r="94" spans="1:8" ht="39" customHeight="1">
       <c r="A94" s="3"/>
@@ -2451,9 +2454,9 @@
       <c r="C94" s="4"/>
       <c r="D94" s="5"/>
       <c r="E94" s="26"/>
-      <c r="F94" s="43"/>
-      <c r="G94" s="44"/>
-      <c r="H94" s="45"/>
+      <c r="F94" s="40"/>
+      <c r="G94" s="41"/>
+      <c r="H94" s="42"/>
     </row>
     <row r="95" spans="1:8" ht="39" customHeight="1">
       <c r="A95" s="3"/>
@@ -2461,9 +2464,9 @@
       <c r="C95" s="4"/>
       <c r="D95" s="5"/>
       <c r="E95" s="26"/>
-      <c r="F95" s="43"/>
-      <c r="G95" s="44"/>
-      <c r="H95" s="45"/>
+      <c r="F95" s="40"/>
+      <c r="G95" s="41"/>
+      <c r="H95" s="42"/>
     </row>
     <row r="96" spans="1:8" ht="39" customHeight="1">
       <c r="A96" s="3"/>
@@ -2471,9 +2474,9 @@
       <c r="C96" s="4"/>
       <c r="D96" s="5"/>
       <c r="E96" s="26"/>
-      <c r="F96" s="43"/>
-      <c r="G96" s="44"/>
-      <c r="H96" s="45"/>
+      <c r="F96" s="40"/>
+      <c r="G96" s="41"/>
+      <c r="H96" s="42"/>
     </row>
     <row r="97" spans="1:8" ht="39" customHeight="1">
       <c r="A97" s="3"/>
@@ -2481,9 +2484,9 @@
       <c r="C97" s="4"/>
       <c r="D97" s="5"/>
       <c r="E97" s="26"/>
-      <c r="F97" s="43"/>
-      <c r="G97" s="44"/>
-      <c r="H97" s="45"/>
+      <c r="F97" s="40"/>
+      <c r="G97" s="41"/>
+      <c r="H97" s="42"/>
     </row>
     <row r="98" spans="1:8" ht="39" customHeight="1">
       <c r="A98" s="3"/>
@@ -2491,9 +2494,9 @@
       <c r="C98" s="4"/>
       <c r="D98" s="5"/>
       <c r="E98" s="26"/>
-      <c r="F98" s="43"/>
-      <c r="G98" s="44"/>
-      <c r="H98" s="45"/>
+      <c r="F98" s="40"/>
+      <c r="G98" s="41"/>
+      <c r="H98" s="42"/>
     </row>
     <row r="99" spans="1:8" ht="39" customHeight="1">
       <c r="A99" s="3"/>
@@ -2501,9 +2504,9 @@
       <c r="C99" s="4"/>
       <c r="D99" s="5"/>
       <c r="E99" s="26"/>
-      <c r="F99" s="43"/>
-      <c r="G99" s="44"/>
-      <c r="H99" s="45"/>
+      <c r="F99" s="40"/>
+      <c r="G99" s="41"/>
+      <c r="H99" s="42"/>
     </row>
     <row r="100" spans="1:8" ht="39" customHeight="1">
       <c r="A100" s="3"/>
@@ -2511,9 +2514,9 @@
       <c r="C100" s="4"/>
       <c r="D100" s="5"/>
       <c r="E100" s="26"/>
-      <c r="F100" s="43"/>
-      <c r="G100" s="44"/>
-      <c r="H100" s="45"/>
+      <c r="F100" s="40"/>
+      <c r="G100" s="41"/>
+      <c r="H100" s="42"/>
     </row>
     <row r="101" spans="1:8" ht="39" customHeight="1">
       <c r="A101" s="3"/>
@@ -2521,9 +2524,9 @@
       <c r="C101" s="4"/>
       <c r="D101" s="5"/>
       <c r="E101" s="26"/>
-      <c r="F101" s="43"/>
-      <c r="G101" s="44"/>
-      <c r="H101" s="45"/>
+      <c r="F101" s="40"/>
+      <c r="G101" s="41"/>
+      <c r="H101" s="42"/>
     </row>
     <row r="102" spans="1:8" ht="39" customHeight="1">
       <c r="A102" s="3"/>
@@ -2531,9 +2534,9 @@
       <c r="C102" s="4"/>
       <c r="D102" s="5"/>
       <c r="E102" s="26"/>
-      <c r="F102" s="43"/>
-      <c r="G102" s="44"/>
-      <c r="H102" s="45"/>
+      <c r="F102" s="40"/>
+      <c r="G102" s="41"/>
+      <c r="H102" s="42"/>
     </row>
     <row r="103" spans="1:8" ht="39" customHeight="1">
       <c r="A103" s="3"/>
@@ -2541,9 +2544,9 @@
       <c r="C103" s="4"/>
       <c r="D103" s="5"/>
       <c r="E103" s="26"/>
-      <c r="F103" s="43"/>
-      <c r="G103" s="44"/>
-      <c r="H103" s="45"/>
+      <c r="F103" s="40"/>
+      <c r="G103" s="41"/>
+      <c r="H103" s="42"/>
     </row>
     <row r="104" spans="1:8" ht="39" customHeight="1">
       <c r="A104" s="3"/>
@@ -2551,9 +2554,9 @@
       <c r="C104" s="4"/>
       <c r="D104" s="5"/>
       <c r="E104" s="26"/>
-      <c r="F104" s="43"/>
-      <c r="G104" s="44"/>
-      <c r="H104" s="45"/>
+      <c r="F104" s="40"/>
+      <c r="G104" s="41"/>
+      <c r="H104" s="42"/>
     </row>
     <row r="105" spans="1:8" ht="39" customHeight="1">
       <c r="A105" s="3"/>
@@ -2561,9 +2564,9 @@
       <c r="C105" s="4"/>
       <c r="D105" s="5"/>
       <c r="E105" s="26"/>
-      <c r="F105" s="43"/>
-      <c r="G105" s="44"/>
-      <c r="H105" s="45"/>
+      <c r="F105" s="40"/>
+      <c r="G105" s="41"/>
+      <c r="H105" s="42"/>
     </row>
     <row r="106" spans="1:8" ht="39" customHeight="1">
       <c r="A106" s="3"/>
@@ -2571,9 +2574,9 @@
       <c r="C106" s="4"/>
       <c r="D106" s="5"/>
       <c r="E106" s="26"/>
-      <c r="F106" s="43"/>
-      <c r="G106" s="44"/>
-      <c r="H106" s="45"/>
+      <c r="F106" s="40"/>
+      <c r="G106" s="41"/>
+      <c r="H106" s="42"/>
     </row>
     <row r="107" spans="1:8" ht="39" customHeight="1">
       <c r="A107" s="3"/>
@@ -2581,9 +2584,9 @@
       <c r="C107" s="4"/>
       <c r="D107" s="5"/>
       <c r="E107" s="26"/>
-      <c r="F107" s="43"/>
-      <c r="G107" s="44"/>
-      <c r="H107" s="45"/>
+      <c r="F107" s="40"/>
+      <c r="G107" s="41"/>
+      <c r="H107" s="42"/>
     </row>
     <row r="108" spans="1:8" ht="39" customHeight="1">
       <c r="A108" s="3"/>
@@ -2591,9 +2594,9 @@
       <c r="C108" s="4"/>
       <c r="D108" s="5"/>
       <c r="E108" s="26"/>
-      <c r="F108" s="43"/>
-      <c r="G108" s="44"/>
-      <c r="H108" s="45"/>
+      <c r="F108" s="40"/>
+      <c r="G108" s="41"/>
+      <c r="H108" s="42"/>
     </row>
     <row r="109" spans="1:8" ht="39" customHeight="1">
       <c r="A109" s="3"/>
@@ -2601,9 +2604,9 @@
       <c r="C109" s="4"/>
       <c r="D109" s="5"/>
       <c r="E109" s="26"/>
-      <c r="F109" s="43"/>
-      <c r="G109" s="44"/>
-      <c r="H109" s="45"/>
+      <c r="F109" s="40"/>
+      <c r="G109" s="41"/>
+      <c r="H109" s="42"/>
     </row>
     <row r="110" spans="1:8" ht="39" customHeight="1">
       <c r="A110" s="3"/>
@@ -2611,9 +2614,9 @@
       <c r="C110" s="4"/>
       <c r="D110" s="5"/>
       <c r="E110" s="26"/>
-      <c r="F110" s="43"/>
-      <c r="G110" s="44"/>
-      <c r="H110" s="45"/>
+      <c r="F110" s="40"/>
+      <c r="G110" s="41"/>
+      <c r="H110" s="42"/>
     </row>
     <row r="111" spans="1:8" ht="39" customHeight="1">
       <c r="A111" s="3"/>
@@ -2621,9 +2624,9 @@
       <c r="C111" s="4"/>
       <c r="D111" s="5"/>
       <c r="E111" s="26"/>
-      <c r="F111" s="43"/>
-      <c r="G111" s="44"/>
-      <c r="H111" s="45"/>
+      <c r="F111" s="40"/>
+      <c r="G111" s="41"/>
+      <c r="H111" s="42"/>
     </row>
     <row r="112" spans="1:8" ht="39" customHeight="1">
       <c r="A112" s="3"/>
@@ -2631,9 +2634,9 @@
       <c r="C112" s="4"/>
       <c r="D112" s="5"/>
       <c r="E112" s="26"/>
-      <c r="F112" s="43"/>
-      <c r="G112" s="44"/>
-      <c r="H112" s="45"/>
+      <c r="F112" s="40"/>
+      <c r="G112" s="41"/>
+      <c r="H112" s="42"/>
     </row>
     <row r="113" spans="1:8" ht="39" customHeight="1">
       <c r="A113" s="3"/>
@@ -2641,9 +2644,9 @@
       <c r="C113" s="4"/>
       <c r="D113" s="5"/>
       <c r="E113" s="26"/>
-      <c r="F113" s="43"/>
-      <c r="G113" s="44"/>
-      <c r="H113" s="45"/>
+      <c r="F113" s="40"/>
+      <c r="G113" s="41"/>
+      <c r="H113" s="42"/>
     </row>
     <row r="114" spans="1:8" ht="39" customHeight="1">
       <c r="A114" s="3"/>
@@ -2651,9 +2654,9 @@
       <c r="C114" s="4"/>
       <c r="D114" s="5"/>
       <c r="E114" s="26"/>
-      <c r="F114" s="43"/>
-      <c r="G114" s="44"/>
-      <c r="H114" s="45"/>
+      <c r="F114" s="40"/>
+      <c r="G114" s="41"/>
+      <c r="H114" s="42"/>
     </row>
     <row r="115" spans="1:8" ht="39" customHeight="1">
       <c r="A115" s="3"/>
@@ -2661,9 +2664,9 @@
       <c r="C115" s="4"/>
       <c r="D115" s="5"/>
       <c r="E115" s="26"/>
-      <c r="F115" s="43"/>
-      <c r="G115" s="44"/>
-      <c r="H115" s="45"/>
+      <c r="F115" s="40"/>
+      <c r="G115" s="41"/>
+      <c r="H115" s="42"/>
     </row>
     <row r="116" spans="1:8" ht="39" customHeight="1">
       <c r="A116" s="3"/>
@@ -2671,9 +2674,9 @@
       <c r="C116" s="4"/>
       <c r="D116" s="5"/>
       <c r="E116" s="26"/>
-      <c r="F116" s="43"/>
-      <c r="G116" s="44"/>
-      <c r="H116" s="45"/>
+      <c r="F116" s="40"/>
+      <c r="G116" s="41"/>
+      <c r="H116" s="42"/>
     </row>
     <row r="117" spans="1:8" ht="39" customHeight="1">
       <c r="A117" s="3"/>
@@ -2681,9 +2684,9 @@
       <c r="C117" s="4"/>
       <c r="D117" s="5"/>
       <c r="E117" s="26"/>
-      <c r="F117" s="43"/>
-      <c r="G117" s="44"/>
-      <c r="H117" s="45"/>
+      <c r="F117" s="40"/>
+      <c r="G117" s="41"/>
+      <c r="H117" s="42"/>
     </row>
     <row r="118" spans="1:8" ht="39" customHeight="1">
       <c r="A118" s="3"/>
@@ -2691,9 +2694,9 @@
       <c r="C118" s="4"/>
       <c r="D118" s="5"/>
       <c r="E118" s="26"/>
-      <c r="F118" s="43"/>
-      <c r="G118" s="44"/>
-      <c r="H118" s="45"/>
+      <c r="F118" s="40"/>
+      <c r="G118" s="41"/>
+      <c r="H118" s="42"/>
     </row>
     <row r="119" spans="1:8" ht="39" customHeight="1">
       <c r="A119" s="3"/>
@@ -2701,9 +2704,9 @@
       <c r="C119" s="4"/>
       <c r="D119" s="5"/>
       <c r="E119" s="26"/>
-      <c r="F119" s="43"/>
-      <c r="G119" s="44"/>
-      <c r="H119" s="45"/>
+      <c r="F119" s="40"/>
+      <c r="G119" s="41"/>
+      <c r="H119" s="42"/>
     </row>
     <row r="120" spans="1:8" ht="39" customHeight="1">
       <c r="A120" s="3"/>
@@ -2711,9 +2714,9 @@
       <c r="C120" s="4"/>
       <c r="D120" s="5"/>
       <c r="E120" s="26"/>
-      <c r="F120" s="43"/>
-      <c r="G120" s="44"/>
-      <c r="H120" s="45"/>
+      <c r="F120" s="40"/>
+      <c r="G120" s="41"/>
+      <c r="H120" s="42"/>
     </row>
     <row r="121" spans="1:8" ht="39" customHeight="1">
       <c r="A121" s="3"/>
@@ -2721,9 +2724,9 @@
       <c r="C121" s="4"/>
       <c r="D121" s="5"/>
       <c r="E121" s="26"/>
-      <c r="F121" s="43"/>
-      <c r="G121" s="44"/>
-      <c r="H121" s="45"/>
+      <c r="F121" s="40"/>
+      <c r="G121" s="41"/>
+      <c r="H121" s="42"/>
     </row>
     <row r="122" spans="1:8" ht="39" customHeight="1">
       <c r="A122" s="3"/>
@@ -2731,9 +2734,9 @@
       <c r="C122" s="4"/>
       <c r="D122" s="5"/>
       <c r="E122" s="26"/>
-      <c r="F122" s="43"/>
-      <c r="G122" s="44"/>
-      <c r="H122" s="45"/>
+      <c r="F122" s="40"/>
+      <c r="G122" s="41"/>
+      <c r="H122" s="42"/>
     </row>
     <row r="123" spans="1:8" ht="39" customHeight="1">
       <c r="A123" s="3"/>
@@ -2741,9 +2744,9 @@
       <c r="C123" s="4"/>
       <c r="D123" s="5"/>
       <c r="E123" s="26"/>
-      <c r="F123" s="43"/>
-      <c r="G123" s="44"/>
-      <c r="H123" s="45"/>
+      <c r="F123" s="40"/>
+      <c r="G123" s="41"/>
+      <c r="H123" s="42"/>
     </row>
     <row r="124" spans="1:8" ht="39" customHeight="1">
       <c r="A124" s="3"/>
@@ -2751,9 +2754,9 @@
       <c r="C124" s="4"/>
       <c r="D124" s="5"/>
       <c r="E124" s="26"/>
-      <c r="F124" s="43"/>
-      <c r="G124" s="44"/>
-      <c r="H124" s="45"/>
+      <c r="F124" s="40"/>
+      <c r="G124" s="41"/>
+      <c r="H124" s="42"/>
     </row>
     <row r="125" spans="1:8" ht="39" customHeight="1">
       <c r="A125" s="3"/>
@@ -2761,9 +2764,9 @@
       <c r="C125" s="4"/>
       <c r="D125" s="5"/>
       <c r="E125" s="26"/>
-      <c r="F125" s="43"/>
-      <c r="G125" s="44"/>
-      <c r="H125" s="45"/>
+      <c r="F125" s="40"/>
+      <c r="G125" s="41"/>
+      <c r="H125" s="42"/>
     </row>
     <row r="126" spans="1:8" ht="39" customHeight="1">
       <c r="A126" s="3"/>
@@ -2771,9 +2774,9 @@
       <c r="C126" s="4"/>
       <c r="D126" s="5"/>
       <c r="E126" s="26"/>
-      <c r="F126" s="43"/>
-      <c r="G126" s="44"/>
-      <c r="H126" s="45"/>
+      <c r="F126" s="40"/>
+      <c r="G126" s="41"/>
+      <c r="H126" s="42"/>
     </row>
     <row r="127" spans="1:8" ht="39" customHeight="1">
       <c r="A127" s="3"/>
@@ -2781,9 +2784,9 @@
       <c r="C127" s="4"/>
       <c r="D127" s="5"/>
       <c r="E127" s="26"/>
-      <c r="F127" s="43"/>
-      <c r="G127" s="44"/>
-      <c r="H127" s="45"/>
+      <c r="F127" s="40"/>
+      <c r="G127" s="41"/>
+      <c r="H127" s="42"/>
     </row>
     <row r="128" spans="1:8" ht="39" customHeight="1">
       <c r="A128" s="3"/>
@@ -2791,9 +2794,9 @@
       <c r="C128" s="4"/>
       <c r="D128" s="5"/>
       <c r="E128" s="26"/>
-      <c r="F128" s="37"/>
-      <c r="G128" s="38"/>
-      <c r="H128" s="39"/>
+      <c r="F128" s="61"/>
+      <c r="G128" s="62"/>
+      <c r="H128" s="63"/>
     </row>
     <row r="129" spans="1:8" ht="39" customHeight="1">
       <c r="A129" s="3"/>
@@ -2801,9 +2804,9 @@
       <c r="C129" s="4"/>
       <c r="D129" s="5"/>
       <c r="E129" s="26"/>
-      <c r="F129" s="37"/>
-      <c r="G129" s="38"/>
-      <c r="H129" s="39"/>
+      <c r="F129" s="61"/>
+      <c r="G129" s="62"/>
+      <c r="H129" s="63"/>
     </row>
     <row r="130" spans="1:8" ht="39" customHeight="1">
       <c r="A130" s="3"/>
@@ -2811,9 +2814,9 @@
       <c r="C130" s="4"/>
       <c r="D130" s="5"/>
       <c r="E130" s="26"/>
-      <c r="F130" s="37"/>
-      <c r="G130" s="38"/>
-      <c r="H130" s="39"/>
+      <c r="F130" s="61"/>
+      <c r="G130" s="62"/>
+      <c r="H130" s="63"/>
     </row>
     <row r="131" spans="1:8" ht="39" customHeight="1">
       <c r="A131" s="3"/>
@@ -2821,9 +2824,9 @@
       <c r="C131" s="4"/>
       <c r="D131" s="5"/>
       <c r="E131" s="26"/>
-      <c r="F131" s="37"/>
-      <c r="G131" s="38"/>
-      <c r="H131" s="39"/>
+      <c r="F131" s="61"/>
+      <c r="G131" s="62"/>
+      <c r="H131" s="63"/>
     </row>
     <row r="132" spans="1:8" ht="39" customHeight="1">
       <c r="A132" s="3"/>
@@ -2831,9 +2834,9 @@
       <c r="C132" s="4"/>
       <c r="D132" s="5"/>
       <c r="E132" s="26"/>
-      <c r="F132" s="37"/>
-      <c r="G132" s="38"/>
-      <c r="H132" s="39"/>
+      <c r="F132" s="61"/>
+      <c r="G132" s="62"/>
+      <c r="H132" s="63"/>
     </row>
     <row r="133" spans="1:8" ht="39" customHeight="1">
       <c r="A133" s="3"/>
@@ -2841,9 +2844,9 @@
       <c r="C133" s="4"/>
       <c r="D133" s="5"/>
       <c r="E133" s="26"/>
-      <c r="F133" s="37"/>
-      <c r="G133" s="38"/>
-      <c r="H133" s="39"/>
+      <c r="F133" s="61"/>
+      <c r="G133" s="62"/>
+      <c r="H133" s="63"/>
     </row>
     <row r="134" spans="1:8" ht="39" customHeight="1">
       <c r="A134" s="3"/>
@@ -2851,9 +2854,9 @@
       <c r="C134" s="4"/>
       <c r="D134" s="5"/>
       <c r="E134" s="26"/>
-      <c r="F134" s="37"/>
-      <c r="G134" s="38"/>
-      <c r="H134" s="39"/>
+      <c r="F134" s="61"/>
+      <c r="G134" s="62"/>
+      <c r="H134" s="63"/>
     </row>
     <row r="135" spans="1:8" ht="39" customHeight="1">
       <c r="A135" s="3"/>
@@ -2861,9 +2864,9 @@
       <c r="C135" s="4"/>
       <c r="D135" s="5"/>
       <c r="E135" s="26"/>
-      <c r="F135" s="37"/>
-      <c r="G135" s="38"/>
-      <c r="H135" s="39"/>
+      <c r="F135" s="61"/>
+      <c r="G135" s="62"/>
+      <c r="H135" s="63"/>
     </row>
     <row r="136" spans="1:8" ht="39" customHeight="1">
       <c r="A136" s="3"/>
@@ -2871,9 +2874,9 @@
       <c r="C136" s="4"/>
       <c r="D136" s="5"/>
       <c r="E136" s="26"/>
-      <c r="F136" s="37"/>
-      <c r="G136" s="38"/>
-      <c r="H136" s="39"/>
+      <c r="F136" s="61"/>
+      <c r="G136" s="62"/>
+      <c r="H136" s="63"/>
     </row>
     <row r="137" spans="1:8" ht="39" customHeight="1">
       <c r="A137" s="3"/>
@@ -2881,9 +2884,9 @@
       <c r="C137" s="4"/>
       <c r="D137" s="5"/>
       <c r="E137" s="26"/>
-      <c r="F137" s="37"/>
-      <c r="G137" s="38"/>
-      <c r="H137" s="39"/>
+      <c r="F137" s="61"/>
+      <c r="G137" s="62"/>
+      <c r="H137" s="63"/>
     </row>
     <row r="138" spans="1:8" ht="39" customHeight="1">
       <c r="A138" s="3"/>
@@ -2891,9 +2894,9 @@
       <c r="C138" s="4"/>
       <c r="D138" s="5"/>
       <c r="E138" s="26"/>
-      <c r="F138" s="37"/>
-      <c r="G138" s="38"/>
-      <c r="H138" s="39"/>
+      <c r="F138" s="61"/>
+      <c r="G138" s="62"/>
+      <c r="H138" s="63"/>
     </row>
     <row r="139" spans="1:8" ht="39" customHeight="1">
       <c r="A139" s="3"/>
@@ -2901,9 +2904,9 @@
       <c r="C139" s="4"/>
       <c r="D139" s="5"/>
       <c r="E139" s="26"/>
-      <c r="F139" s="37"/>
-      <c r="G139" s="38"/>
-      <c r="H139" s="39"/>
+      <c r="F139" s="61"/>
+      <c r="G139" s="62"/>
+      <c r="H139" s="63"/>
     </row>
     <row r="140" spans="1:8" ht="39" customHeight="1">
       <c r="A140" s="3"/>
@@ -2911,9 +2914,9 @@
       <c r="C140" s="4"/>
       <c r="D140" s="5"/>
       <c r="E140" s="26"/>
-      <c r="F140" s="37"/>
-      <c r="G140" s="38"/>
-      <c r="H140" s="39"/>
+      <c r="F140" s="61"/>
+      <c r="G140" s="62"/>
+      <c r="H140" s="63"/>
     </row>
     <row r="141" spans="1:8" ht="39" customHeight="1">
       <c r="A141" s="3"/>
@@ -2921,9 +2924,9 @@
       <c r="C141" s="4"/>
       <c r="D141" s="5"/>
       <c r="E141" s="26"/>
-      <c r="F141" s="37"/>
-      <c r="G141" s="38"/>
-      <c r="H141" s="39"/>
+      <c r="F141" s="61"/>
+      <c r="G141" s="62"/>
+      <c r="H141" s="63"/>
     </row>
     <row r="142" spans="1:8" ht="39" customHeight="1">
       <c r="A142" s="3"/>
@@ -2931,9 +2934,9 @@
       <c r="C142" s="4"/>
       <c r="D142" s="5"/>
       <c r="E142" s="26"/>
-      <c r="F142" s="37"/>
-      <c r="G142" s="38"/>
-      <c r="H142" s="39"/>
+      <c r="F142" s="61"/>
+      <c r="G142" s="62"/>
+      <c r="H142" s="63"/>
     </row>
     <row r="143" spans="1:8" ht="39" customHeight="1">
       <c r="A143" s="3"/>
@@ -2941,9 +2944,9 @@
       <c r="C143" s="4"/>
       <c r="D143" s="5"/>
       <c r="E143" s="26"/>
-      <c r="F143" s="37"/>
-      <c r="G143" s="38"/>
-      <c r="H143" s="39"/>
+      <c r="F143" s="61"/>
+      <c r="G143" s="62"/>
+      <c r="H143" s="63"/>
     </row>
     <row r="144" spans="1:8" ht="39" customHeight="1">
       <c r="A144" s="3"/>
@@ -2951,9 +2954,9 @@
       <c r="C144" s="4"/>
       <c r="D144" s="5"/>
       <c r="E144" s="26"/>
-      <c r="F144" s="37"/>
-      <c r="G144" s="38"/>
-      <c r="H144" s="39"/>
+      <c r="F144" s="61"/>
+      <c r="G144" s="62"/>
+      <c r="H144" s="63"/>
     </row>
     <row r="145" spans="1:8" ht="39" customHeight="1">
       <c r="A145" s="3"/>
@@ -2961,9 +2964,9 @@
       <c r="C145" s="4"/>
       <c r="D145" s="5"/>
       <c r="E145" s="26"/>
-      <c r="F145" s="37"/>
-      <c r="G145" s="38"/>
-      <c r="H145" s="39"/>
+      <c r="F145" s="61"/>
+      <c r="G145" s="62"/>
+      <c r="H145" s="63"/>
     </row>
     <row r="146" spans="1:8" ht="39" customHeight="1">
       <c r="A146" s="3"/>
@@ -2971,9 +2974,9 @@
       <c r="C146" s="4"/>
       <c r="D146" s="5"/>
       <c r="E146" s="26"/>
-      <c r="F146" s="37"/>
-      <c r="G146" s="38"/>
-      <c r="H146" s="39"/>
+      <c r="F146" s="61"/>
+      <c r="G146" s="62"/>
+      <c r="H146" s="63"/>
     </row>
     <row r="147" spans="1:8" ht="39" customHeight="1">
       <c r="A147" s="3"/>
@@ -2981,9 +2984,9 @@
       <c r="C147" s="4"/>
       <c r="D147" s="5"/>
       <c r="E147" s="26"/>
-      <c r="F147" s="37"/>
-      <c r="G147" s="38"/>
-      <c r="H147" s="39"/>
+      <c r="F147" s="61"/>
+      <c r="G147" s="62"/>
+      <c r="H147" s="63"/>
     </row>
     <row r="148" spans="1:8" ht="39" customHeight="1">
       <c r="A148" s="3"/>
@@ -2991,9 +2994,9 @@
       <c r="C148" s="4"/>
       <c r="D148" s="5"/>
       <c r="E148" s="26"/>
-      <c r="F148" s="37"/>
-      <c r="G148" s="38"/>
-      <c r="H148" s="39"/>
+      <c r="F148" s="61"/>
+      <c r="G148" s="62"/>
+      <c r="H148" s="63"/>
     </row>
     <row r="149" spans="1:8" ht="39" customHeight="1">
       <c r="A149" s="3"/>
@@ -3001,9 +3004,9 @@
       <c r="C149" s="4"/>
       <c r="D149" s="5"/>
       <c r="E149" s="26"/>
-      <c r="F149" s="37"/>
-      <c r="G149" s="38"/>
-      <c r="H149" s="39"/>
+      <c r="F149" s="61"/>
+      <c r="G149" s="62"/>
+      <c r="H149" s="63"/>
     </row>
     <row r="150" spans="1:8" ht="39" customHeight="1">
       <c r="A150" s="3"/>
@@ -3011,9 +3014,9 @@
       <c r="C150" s="4"/>
       <c r="D150" s="5"/>
       <c r="E150" s="26"/>
-      <c r="F150" s="37"/>
-      <c r="G150" s="38"/>
-      <c r="H150" s="39"/>
+      <c r="F150" s="61"/>
+      <c r="G150" s="62"/>
+      <c r="H150" s="63"/>
     </row>
     <row r="151" spans="1:8" ht="39" customHeight="1">
       <c r="A151" s="3"/>
@@ -3021,9 +3024,9 @@
       <c r="C151" s="4"/>
       <c r="D151" s="5"/>
       <c r="E151" s="26"/>
-      <c r="F151" s="37"/>
-      <c r="G151" s="38"/>
-      <c r="H151" s="39"/>
+      <c r="F151" s="61"/>
+      <c r="G151" s="62"/>
+      <c r="H151" s="63"/>
     </row>
     <row r="152" spans="1:8" ht="39" customHeight="1">
       <c r="A152" s="3"/>
@@ -3031,9 +3034,9 @@
       <c r="C152" s="4"/>
       <c r="D152" s="5"/>
       <c r="E152" s="26"/>
-      <c r="F152" s="37"/>
-      <c r="G152" s="38"/>
-      <c r="H152" s="39"/>
+      <c r="F152" s="61"/>
+      <c r="G152" s="62"/>
+      <c r="H152" s="63"/>
     </row>
     <row r="153" spans="1:8" ht="39" customHeight="1">
       <c r="A153" s="3"/>
@@ -3041,9 +3044,9 @@
       <c r="C153" s="4"/>
       <c r="D153" s="5"/>
       <c r="E153" s="26"/>
-      <c r="F153" s="37"/>
-      <c r="G153" s="38"/>
-      <c r="H153" s="39"/>
+      <c r="F153" s="61"/>
+      <c r="G153" s="62"/>
+      <c r="H153" s="63"/>
     </row>
     <row r="154" spans="1:8" ht="39" customHeight="1">
       <c r="A154" s="3"/>
@@ -3051,9 +3054,9 @@
       <c r="C154" s="4"/>
       <c r="D154" s="5"/>
       <c r="E154" s="26"/>
-      <c r="F154" s="37"/>
-      <c r="G154" s="38"/>
-      <c r="H154" s="39"/>
+      <c r="F154" s="61"/>
+      <c r="G154" s="62"/>
+      <c r="H154" s="63"/>
     </row>
     <row r="155" spans="1:8" ht="39" customHeight="1">
       <c r="A155" s="3"/>
@@ -3061,9 +3064,9 @@
       <c r="C155" s="4"/>
       <c r="D155" s="5"/>
       <c r="E155" s="26"/>
-      <c r="F155" s="37"/>
-      <c r="G155" s="38"/>
-      <c r="H155" s="39"/>
+      <c r="F155" s="61"/>
+      <c r="G155" s="62"/>
+      <c r="H155" s="63"/>
     </row>
     <row r="156" spans="1:8" ht="39" customHeight="1">
       <c r="A156" s="3"/>
@@ -3071,9 +3074,9 @@
       <c r="C156" s="4"/>
       <c r="D156" s="5"/>
       <c r="E156" s="26"/>
-      <c r="F156" s="37"/>
-      <c r="G156" s="38"/>
-      <c r="H156" s="39"/>
+      <c r="F156" s="61"/>
+      <c r="G156" s="62"/>
+      <c r="H156" s="63"/>
     </row>
     <row r="157" spans="1:8" ht="39" customHeight="1">
       <c r="A157" s="3"/>
@@ -3081,9 +3084,9 @@
       <c r="C157" s="4"/>
       <c r="D157" s="5"/>
       <c r="E157" s="26"/>
-      <c r="F157" s="37"/>
-      <c r="G157" s="38"/>
-      <c r="H157" s="39"/>
+      <c r="F157" s="61"/>
+      <c r="G157" s="62"/>
+      <c r="H157" s="63"/>
     </row>
     <row r="158" spans="1:8" ht="39" customHeight="1">
       <c r="A158" s="3"/>
@@ -3091,9 +3094,9 @@
       <c r="C158" s="4"/>
       <c r="D158" s="5"/>
       <c r="E158" s="26"/>
-      <c r="F158" s="37"/>
-      <c r="G158" s="38"/>
-      <c r="H158" s="39"/>
+      <c r="F158" s="61"/>
+      <c r="G158" s="62"/>
+      <c r="H158" s="63"/>
     </row>
     <row r="159" spans="1:8" ht="39" customHeight="1">
       <c r="A159" s="3"/>
@@ -3101,9 +3104,9 @@
       <c r="C159" s="4"/>
       <c r="D159" s="5"/>
       <c r="E159" s="26"/>
-      <c r="F159" s="37"/>
-      <c r="G159" s="38"/>
-      <c r="H159" s="39"/>
+      <c r="F159" s="61"/>
+      <c r="G159" s="62"/>
+      <c r="H159" s="63"/>
     </row>
     <row r="160" spans="1:8" ht="39" customHeight="1">
       <c r="A160" s="3"/>
@@ -3111,9 +3114,9 @@
       <c r="C160" s="4"/>
       <c r="D160" s="5"/>
       <c r="E160" s="26"/>
-      <c r="F160" s="37"/>
-      <c r="G160" s="38"/>
-      <c r="H160" s="39"/>
+      <c r="F160" s="61"/>
+      <c r="G160" s="62"/>
+      <c r="H160" s="63"/>
     </row>
     <row r="161" spans="1:8" ht="39" customHeight="1">
       <c r="A161" s="3"/>
@@ -3121,9 +3124,9 @@
       <c r="C161" s="4"/>
       <c r="D161" s="5"/>
       <c r="E161" s="26"/>
-      <c r="F161" s="37"/>
-      <c r="G161" s="38"/>
-      <c r="H161" s="39"/>
+      <c r="F161" s="61"/>
+      <c r="G161" s="62"/>
+      <c r="H161" s="63"/>
     </row>
     <row r="162" spans="1:8" ht="39" customHeight="1">
       <c r="A162" s="3"/>
@@ -3131,9 +3134,9 @@
       <c r="C162" s="4"/>
       <c r="D162" s="5"/>
       <c r="E162" s="26"/>
-      <c r="F162" s="37"/>
-      <c r="G162" s="38"/>
-      <c r="H162" s="39"/>
+      <c r="F162" s="61"/>
+      <c r="G162" s="62"/>
+      <c r="H162" s="63"/>
     </row>
     <row r="163" spans="1:8" ht="39" customHeight="1">
       <c r="A163" s="3"/>
@@ -3141,9 +3144,9 @@
       <c r="C163" s="4"/>
       <c r="D163" s="5"/>
       <c r="E163" s="26"/>
-      <c r="F163" s="37"/>
-      <c r="G163" s="38"/>
-      <c r="H163" s="39"/>
+      <c r="F163" s="61"/>
+      <c r="G163" s="62"/>
+      <c r="H163" s="63"/>
     </row>
     <row r="164" spans="1:8" ht="39" customHeight="1">
       <c r="A164" s="3"/>
@@ -3151,9 +3154,9 @@
       <c r="C164" s="4"/>
       <c r="D164" s="5"/>
       <c r="E164" s="26"/>
-      <c r="F164" s="37"/>
-      <c r="G164" s="38"/>
-      <c r="H164" s="39"/>
+      <c r="F164" s="61"/>
+      <c r="G164" s="62"/>
+      <c r="H164" s="63"/>
     </row>
     <row r="165" spans="1:8" ht="39" customHeight="1">
       <c r="A165" s="3"/>
@@ -3161,9 +3164,9 @@
       <c r="C165" s="4"/>
       <c r="D165" s="5"/>
       <c r="E165" s="26"/>
-      <c r="F165" s="37"/>
-      <c r="G165" s="38"/>
-      <c r="H165" s="39"/>
+      <c r="F165" s="61"/>
+      <c r="G165" s="62"/>
+      <c r="H165" s="63"/>
     </row>
     <row r="166" spans="1:8" ht="39" customHeight="1">
       <c r="A166" s="3"/>
@@ -3171,9 +3174,9 @@
       <c r="C166" s="4"/>
       <c r="D166" s="5"/>
       <c r="E166" s="26"/>
-      <c r="F166" s="37"/>
-      <c r="G166" s="38"/>
-      <c r="H166" s="39"/>
+      <c r="F166" s="61"/>
+      <c r="G166" s="62"/>
+      <c r="H166" s="63"/>
     </row>
     <row r="167" spans="1:8" ht="39" customHeight="1">
       <c r="A167" s="3"/>
@@ -3181,9 +3184,9 @@
       <c r="C167" s="4"/>
       <c r="D167" s="5"/>
       <c r="E167" s="26"/>
-      <c r="F167" s="37"/>
-      <c r="G167" s="38"/>
-      <c r="H167" s="39"/>
+      <c r="F167" s="61"/>
+      <c r="G167" s="62"/>
+      <c r="H167" s="63"/>
     </row>
     <row r="168" spans="1:8" ht="39" customHeight="1">
       <c r="A168" s="3"/>
@@ -3191,9 +3194,9 @@
       <c r="C168" s="4"/>
       <c r="D168" s="5"/>
       <c r="E168" s="26"/>
-      <c r="F168" s="37"/>
-      <c r="G168" s="38"/>
-      <c r="H168" s="39"/>
+      <c r="F168" s="61"/>
+      <c r="G168" s="62"/>
+      <c r="H168" s="63"/>
     </row>
     <row r="169" spans="1:8" ht="39" customHeight="1">
       <c r="A169" s="3"/>
@@ -3201,9 +3204,9 @@
       <c r="C169" s="4"/>
       <c r="D169" s="5"/>
       <c r="E169" s="26"/>
-      <c r="F169" s="37"/>
-      <c r="G169" s="38"/>
-      <c r="H169" s="39"/>
+      <c r="F169" s="61"/>
+      <c r="G169" s="62"/>
+      <c r="H169" s="63"/>
     </row>
     <row r="170" spans="1:8" ht="39" customHeight="1">
       <c r="A170" s="3"/>
@@ -3211,9 +3214,9 @@
       <c r="C170" s="4"/>
       <c r="D170" s="5"/>
       <c r="E170" s="26"/>
-      <c r="F170" s="37"/>
-      <c r="G170" s="38"/>
-      <c r="H170" s="39"/>
+      <c r="F170" s="61"/>
+      <c r="G170" s="62"/>
+      <c r="H170" s="63"/>
     </row>
     <row r="171" spans="1:8" ht="39" customHeight="1">
       <c r="A171" s="3"/>
@@ -3221,9 +3224,9 @@
       <c r="C171" s="4"/>
       <c r="D171" s="5"/>
       <c r="E171" s="26"/>
-      <c r="F171" s="37"/>
-      <c r="G171" s="38"/>
-      <c r="H171" s="39"/>
+      <c r="F171" s="61"/>
+      <c r="G171" s="62"/>
+      <c r="H171" s="63"/>
     </row>
     <row r="172" spans="1:8" ht="39" customHeight="1">
       <c r="A172" s="3"/>
@@ -3231,9 +3234,9 @@
       <c r="C172" s="4"/>
       <c r="D172" s="5"/>
       <c r="E172" s="26"/>
-      <c r="F172" s="37"/>
-      <c r="G172" s="38"/>
-      <c r="H172" s="39"/>
+      <c r="F172" s="61"/>
+      <c r="G172" s="62"/>
+      <c r="H172" s="63"/>
     </row>
     <row r="173" spans="1:8" ht="39" customHeight="1">
       <c r="A173" s="3"/>
@@ -3241,9 +3244,9 @@
       <c r="C173" s="4"/>
       <c r="D173" s="5"/>
       <c r="E173" s="26"/>
-      <c r="F173" s="37"/>
-      <c r="G173" s="38"/>
-      <c r="H173" s="39"/>
+      <c r="F173" s="61"/>
+      <c r="G173" s="62"/>
+      <c r="H173" s="63"/>
     </row>
     <row r="174" spans="1:8" ht="39" customHeight="1">
       <c r="A174" s="3"/>
@@ -3251,9 +3254,9 @@
       <c r="C174" s="4"/>
       <c r="D174" s="5"/>
       <c r="E174" s="26"/>
-      <c r="F174" s="37"/>
-      <c r="G174" s="38"/>
-      <c r="H174" s="39"/>
+      <c r="F174" s="61"/>
+      <c r="G174" s="62"/>
+      <c r="H174" s="63"/>
     </row>
     <row r="175" spans="1:8" ht="39" customHeight="1">
       <c r="A175" s="3"/>
@@ -3261,9 +3264,9 @@
       <c r="C175" s="4"/>
       <c r="D175" s="5"/>
       <c r="E175" s="26"/>
-      <c r="F175" s="37"/>
-      <c r="G175" s="38"/>
-      <c r="H175" s="39"/>
+      <c r="F175" s="61"/>
+      <c r="G175" s="62"/>
+      <c r="H175" s="63"/>
     </row>
     <row r="176" spans="1:8" ht="39" customHeight="1">
       <c r="A176" s="3"/>
@@ -3271,9 +3274,9 @@
       <c r="C176" s="4"/>
       <c r="D176" s="5"/>
       <c r="E176" s="26"/>
-      <c r="F176" s="37"/>
-      <c r="G176" s="38"/>
-      <c r="H176" s="39"/>
+      <c r="F176" s="61"/>
+      <c r="G176" s="62"/>
+      <c r="H176" s="63"/>
     </row>
     <row r="177" spans="1:8" ht="39" customHeight="1">
       <c r="A177" s="3"/>
@@ -3281,9 +3284,9 @@
       <c r="C177" s="4"/>
       <c r="D177" s="5"/>
       <c r="E177" s="26"/>
-      <c r="F177" s="37"/>
-      <c r="G177" s="38"/>
-      <c r="H177" s="39"/>
+      <c r="F177" s="61"/>
+      <c r="G177" s="62"/>
+      <c r="H177" s="63"/>
     </row>
     <row r="178" spans="1:8" ht="39" customHeight="1">
       <c r="A178" s="3"/>
@@ -3291,9 +3294,9 @@
       <c r="C178" s="4"/>
       <c r="D178" s="5"/>
       <c r="E178" s="26"/>
-      <c r="F178" s="37"/>
-      <c r="G178" s="38"/>
-      <c r="H178" s="39"/>
+      <c r="F178" s="61"/>
+      <c r="G178" s="62"/>
+      <c r="H178" s="63"/>
     </row>
     <row r="179" spans="1:8" ht="39" customHeight="1">
       <c r="A179" s="3"/>
@@ -3301,9 +3304,9 @@
       <c r="C179" s="4"/>
       <c r="D179" s="5"/>
       <c r="E179" s="26"/>
-      <c r="F179" s="37"/>
-      <c r="G179" s="38"/>
-      <c r="H179" s="39"/>
+      <c r="F179" s="61"/>
+      <c r="G179" s="62"/>
+      <c r="H179" s="63"/>
     </row>
     <row r="180" spans="1:8" ht="39" customHeight="1">
       <c r="A180" s="3"/>
@@ -3311,9 +3314,9 @@
       <c r="C180" s="4"/>
       <c r="D180" s="5"/>
       <c r="E180" s="26"/>
-      <c r="F180" s="37"/>
-      <c r="G180" s="38"/>
-      <c r="H180" s="39"/>
+      <c r="F180" s="61"/>
+      <c r="G180" s="62"/>
+      <c r="H180" s="63"/>
     </row>
     <row r="181" spans="1:8" ht="39" customHeight="1">
       <c r="A181" s="3"/>
@@ -3321,9 +3324,9 @@
       <c r="C181" s="4"/>
       <c r="D181" s="5"/>
       <c r="E181" s="26"/>
-      <c r="F181" s="37"/>
-      <c r="G181" s="38"/>
-      <c r="H181" s="39"/>
+      <c r="F181" s="61"/>
+      <c r="G181" s="62"/>
+      <c r="H181" s="63"/>
     </row>
     <row r="182" spans="1:8" ht="39" customHeight="1">
       <c r="A182" s="3"/>
@@ -3331,9 +3334,9 @@
       <c r="C182" s="4"/>
       <c r="D182" s="5"/>
       <c r="E182" s="26"/>
-      <c r="F182" s="37"/>
-      <c r="G182" s="38"/>
-      <c r="H182" s="39"/>
+      <c r="F182" s="61"/>
+      <c r="G182" s="62"/>
+      <c r="H182" s="63"/>
     </row>
     <row r="183" spans="1:8" ht="39" customHeight="1">
       <c r="A183" s="3"/>
@@ -3341,9 +3344,9 @@
       <c r="C183" s="4"/>
       <c r="D183" s="5"/>
       <c r="E183" s="26"/>
-      <c r="F183" s="37"/>
-      <c r="G183" s="38"/>
-      <c r="H183" s="39"/>
+      <c r="F183" s="61"/>
+      <c r="G183" s="62"/>
+      <c r="H183" s="63"/>
     </row>
     <row r="184" spans="1:8" ht="39" customHeight="1">
       <c r="A184" s="3"/>
@@ -3351,9 +3354,9 @@
       <c r="C184" s="4"/>
       <c r="D184" s="5"/>
       <c r="E184" s="26"/>
-      <c r="F184" s="37"/>
-      <c r="G184" s="38"/>
-      <c r="H184" s="39"/>
+      <c r="F184" s="61"/>
+      <c r="G184" s="62"/>
+      <c r="H184" s="63"/>
     </row>
     <row r="185" spans="1:8" ht="39" customHeight="1">
       <c r="A185" s="3"/>
@@ -3361,9 +3364,9 @@
       <c r="C185" s="4"/>
       <c r="D185" s="5"/>
       <c r="E185" s="26"/>
-      <c r="F185" s="37"/>
-      <c r="G185" s="38"/>
-      <c r="H185" s="39"/>
+      <c r="F185" s="61"/>
+      <c r="G185" s="62"/>
+      <c r="H185" s="63"/>
     </row>
     <row r="186" spans="1:8" ht="39" customHeight="1">
       <c r="A186" s="3"/>
@@ -3371,9 +3374,9 @@
       <c r="C186" s="4"/>
       <c r="D186" s="5"/>
       <c r="E186" s="26"/>
-      <c r="F186" s="37"/>
-      <c r="G186" s="38"/>
-      <c r="H186" s="39"/>
+      <c r="F186" s="61"/>
+      <c r="G186" s="62"/>
+      <c r="H186" s="63"/>
     </row>
     <row r="187" spans="1:8" ht="39" customHeight="1">
       <c r="A187" s="3"/>
@@ -3381,9 +3384,9 @@
       <c r="C187" s="4"/>
       <c r="D187" s="5"/>
       <c r="E187" s="26"/>
-      <c r="F187" s="37"/>
-      <c r="G187" s="38"/>
-      <c r="H187" s="39"/>
+      <c r="F187" s="61"/>
+      <c r="G187" s="62"/>
+      <c r="H187" s="63"/>
     </row>
     <row r="188" spans="1:8" ht="39" customHeight="1">
       <c r="A188" s="3"/>
@@ -3391,9 +3394,9 @@
       <c r="C188" s="4"/>
       <c r="D188" s="5"/>
       <c r="E188" s="26"/>
-      <c r="F188" s="37"/>
-      <c r="G188" s="38"/>
-      <c r="H188" s="39"/>
+      <c r="F188" s="61"/>
+      <c r="G188" s="62"/>
+      <c r="H188" s="63"/>
     </row>
     <row r="189" spans="1:8" ht="39" customHeight="1">
       <c r="A189" s="3"/>
@@ -3401,9 +3404,9 @@
       <c r="C189" s="4"/>
       <c r="D189" s="5"/>
       <c r="E189" s="26"/>
-      <c r="F189" s="37"/>
-      <c r="G189" s="38"/>
-      <c r="H189" s="39"/>
+      <c r="F189" s="61"/>
+      <c r="G189" s="62"/>
+      <c r="H189" s="63"/>
     </row>
     <row r="190" spans="1:8" ht="39" customHeight="1">
       <c r="A190" s="3"/>
@@ -3411,9 +3414,9 @@
       <c r="C190" s="4"/>
       <c r="D190" s="5"/>
       <c r="E190" s="26"/>
-      <c r="F190" s="37"/>
-      <c r="G190" s="38"/>
-      <c r="H190" s="39"/>
+      <c r="F190" s="61"/>
+      <c r="G190" s="62"/>
+      <c r="H190" s="63"/>
     </row>
     <row r="191" spans="1:8" ht="39" customHeight="1">
       <c r="A191" s="3"/>
@@ -3421,9 +3424,9 @@
       <c r="C191" s="4"/>
       <c r="D191" s="5"/>
       <c r="E191" s="26"/>
-      <c r="F191" s="37"/>
-      <c r="G191" s="38"/>
-      <c r="H191" s="39"/>
+      <c r="F191" s="61"/>
+      <c r="G191" s="62"/>
+      <c r="H191" s="63"/>
     </row>
     <row r="192" spans="1:8" ht="39" customHeight="1">
       <c r="A192" s="3"/>
@@ -3431,9 +3434,9 @@
       <c r="C192" s="4"/>
       <c r="D192" s="5"/>
       <c r="E192" s="26"/>
-      <c r="F192" s="37"/>
-      <c r="G192" s="38"/>
-      <c r="H192" s="39"/>
+      <c r="F192" s="61"/>
+      <c r="G192" s="62"/>
+      <c r="H192" s="63"/>
     </row>
     <row r="193" spans="1:8" ht="39" customHeight="1">
       <c r="A193" s="3"/>
@@ -3441,9 +3444,9 @@
       <c r="C193" s="4"/>
       <c r="D193" s="5"/>
       <c r="E193" s="26"/>
-      <c r="F193" s="37"/>
-      <c r="G193" s="38"/>
-      <c r="H193" s="39"/>
+      <c r="F193" s="61"/>
+      <c r="G193" s="62"/>
+      <c r="H193" s="63"/>
     </row>
     <row r="194" spans="1:8" ht="39" customHeight="1">
       <c r="A194" s="3"/>
@@ -3451,9 +3454,9 @@
       <c r="C194" s="4"/>
       <c r="D194" s="5"/>
       <c r="E194" s="26"/>
-      <c r="F194" s="37"/>
-      <c r="G194" s="38"/>
-      <c r="H194" s="39"/>
+      <c r="F194" s="61"/>
+      <c r="G194" s="62"/>
+      <c r="H194" s="63"/>
     </row>
     <row r="195" spans="1:8" ht="39" customHeight="1">
       <c r="A195" s="3"/>
@@ -3461,9 +3464,9 @@
       <c r="C195" s="4"/>
       <c r="D195" s="5"/>
       <c r="E195" s="26"/>
-      <c r="F195" s="37"/>
-      <c r="G195" s="38"/>
-      <c r="H195" s="39"/>
+      <c r="F195" s="61"/>
+      <c r="G195" s="62"/>
+      <c r="H195" s="63"/>
     </row>
     <row r="196" spans="1:8" ht="39" customHeight="1">
       <c r="A196" s="3"/>
@@ -3471,9 +3474,9 @@
       <c r="C196" s="4"/>
       <c r="D196" s="5"/>
       <c r="E196" s="26"/>
-      <c r="F196" s="37"/>
-      <c r="G196" s="38"/>
-      <c r="H196" s="39"/>
+      <c r="F196" s="61"/>
+      <c r="G196" s="62"/>
+      <c r="H196" s="63"/>
     </row>
     <row r="197" spans="1:8" ht="39" customHeight="1">
       <c r="A197" s="3"/>
@@ -3481,9 +3484,9 @@
       <c r="C197" s="4"/>
       <c r="D197" s="5"/>
       <c r="E197" s="26"/>
-      <c r="F197" s="37"/>
-      <c r="G197" s="38"/>
-      <c r="H197" s="39"/>
+      <c r="F197" s="61"/>
+      <c r="G197" s="62"/>
+      <c r="H197" s="63"/>
     </row>
     <row r="198" spans="1:8" ht="39" customHeight="1">
       <c r="A198" s="3"/>
@@ -3491,9 +3494,9 @@
       <c r="C198" s="4"/>
       <c r="D198" s="5"/>
       <c r="E198" s="26"/>
-      <c r="F198" s="37"/>
-      <c r="G198" s="38"/>
-      <c r="H198" s="39"/>
+      <c r="F198" s="61"/>
+      <c r="G198" s="62"/>
+      <c r="H198" s="63"/>
     </row>
     <row r="199" spans="1:8" ht="39" customHeight="1">
       <c r="A199" s="3"/>
@@ -3501,9 +3504,9 @@
       <c r="C199" s="4"/>
       <c r="D199" s="5"/>
       <c r="E199" s="26"/>
-      <c r="F199" s="37"/>
-      <c r="G199" s="38"/>
-      <c r="H199" s="39"/>
+      <c r="F199" s="61"/>
+      <c r="G199" s="62"/>
+      <c r="H199" s="63"/>
     </row>
     <row r="200" spans="1:8" ht="39" customHeight="1" thickBot="1">
       <c r="A200" s="6"/>
@@ -3511,13 +3514,203 @@
       <c r="C200" s="7"/>
       <c r="D200" s="8"/>
       <c r="E200" s="28"/>
-      <c r="F200" s="40"/>
-      <c r="G200" s="41"/>
-      <c r="H200" s="42"/>
+      <c r="F200" s="64"/>
+      <c r="G200" s="65"/>
+      <c r="H200" s="66"/>
     </row>
     <row r="201" spans="1:8" ht="39" hidden="1" customHeight="1" thickTop="1"/>
   </sheetData>
   <mergeCells count="204">
+    <mergeCell ref="F196:H196"/>
+    <mergeCell ref="F197:H197"/>
+    <mergeCell ref="F198:H198"/>
+    <mergeCell ref="F199:H199"/>
+    <mergeCell ref="F200:H200"/>
+    <mergeCell ref="F191:H191"/>
+    <mergeCell ref="F192:H192"/>
+    <mergeCell ref="F193:H193"/>
+    <mergeCell ref="F194:H194"/>
+    <mergeCell ref="F195:H195"/>
+    <mergeCell ref="F186:H186"/>
+    <mergeCell ref="F187:H187"/>
+    <mergeCell ref="F188:H188"/>
+    <mergeCell ref="F189:H189"/>
+    <mergeCell ref="F190:H190"/>
+    <mergeCell ref="F181:H181"/>
+    <mergeCell ref="F182:H182"/>
+    <mergeCell ref="F183:H183"/>
+    <mergeCell ref="F184:H184"/>
+    <mergeCell ref="F185:H185"/>
+    <mergeCell ref="F176:H176"/>
+    <mergeCell ref="F177:H177"/>
+    <mergeCell ref="F178:H178"/>
+    <mergeCell ref="F179:H179"/>
+    <mergeCell ref="F180:H180"/>
+    <mergeCell ref="F171:H171"/>
+    <mergeCell ref="F172:H172"/>
+    <mergeCell ref="F173:H173"/>
+    <mergeCell ref="F174:H174"/>
+    <mergeCell ref="F175:H175"/>
+    <mergeCell ref="F166:H166"/>
+    <mergeCell ref="F167:H167"/>
+    <mergeCell ref="F168:H168"/>
+    <mergeCell ref="F169:H169"/>
+    <mergeCell ref="F170:H170"/>
+    <mergeCell ref="F161:H161"/>
+    <mergeCell ref="F162:H162"/>
+    <mergeCell ref="F163:H163"/>
+    <mergeCell ref="F164:H164"/>
+    <mergeCell ref="F165:H165"/>
+    <mergeCell ref="F156:H156"/>
+    <mergeCell ref="F157:H157"/>
+    <mergeCell ref="F158:H158"/>
+    <mergeCell ref="F159:H159"/>
+    <mergeCell ref="F160:H160"/>
+    <mergeCell ref="F151:H151"/>
+    <mergeCell ref="F152:H152"/>
+    <mergeCell ref="F153:H153"/>
+    <mergeCell ref="F154:H154"/>
+    <mergeCell ref="F155:H155"/>
+    <mergeCell ref="F146:H146"/>
+    <mergeCell ref="F147:H147"/>
+    <mergeCell ref="F148:H148"/>
+    <mergeCell ref="F149:H149"/>
+    <mergeCell ref="F150:H150"/>
+    <mergeCell ref="F141:H141"/>
+    <mergeCell ref="F142:H142"/>
+    <mergeCell ref="F143:H143"/>
+    <mergeCell ref="F144:H144"/>
+    <mergeCell ref="F145:H145"/>
+    <mergeCell ref="F136:H136"/>
+    <mergeCell ref="F137:H137"/>
+    <mergeCell ref="F138:H138"/>
+    <mergeCell ref="F139:H139"/>
+    <mergeCell ref="F140:H140"/>
+    <mergeCell ref="F131:H131"/>
+    <mergeCell ref="F132:H132"/>
+    <mergeCell ref="F133:H133"/>
+    <mergeCell ref="F134:H134"/>
+    <mergeCell ref="F135:H135"/>
+    <mergeCell ref="F126:H126"/>
+    <mergeCell ref="F127:H127"/>
+    <mergeCell ref="F128:H128"/>
+    <mergeCell ref="F129:H129"/>
+    <mergeCell ref="F130:H130"/>
+    <mergeCell ref="F121:H121"/>
+    <mergeCell ref="F122:H122"/>
+    <mergeCell ref="F123:H123"/>
+    <mergeCell ref="F124:H124"/>
+    <mergeCell ref="F125:H125"/>
+    <mergeCell ref="F116:H116"/>
+    <mergeCell ref="F117:H117"/>
+    <mergeCell ref="F118:H118"/>
+    <mergeCell ref="F119:H119"/>
+    <mergeCell ref="F120:H120"/>
+    <mergeCell ref="F111:H111"/>
+    <mergeCell ref="F112:H112"/>
+    <mergeCell ref="F113:H113"/>
+    <mergeCell ref="F114:H114"/>
+    <mergeCell ref="F115:H115"/>
+    <mergeCell ref="F106:H106"/>
+    <mergeCell ref="F107:H107"/>
+    <mergeCell ref="F108:H108"/>
+    <mergeCell ref="F109:H109"/>
+    <mergeCell ref="F110:H110"/>
+    <mergeCell ref="F101:H101"/>
+    <mergeCell ref="F102:H102"/>
+    <mergeCell ref="F103:H103"/>
+    <mergeCell ref="F104:H104"/>
+    <mergeCell ref="F105:H105"/>
+    <mergeCell ref="F96:H96"/>
+    <mergeCell ref="F97:H97"/>
+    <mergeCell ref="F98:H98"/>
+    <mergeCell ref="F99:H99"/>
+    <mergeCell ref="F100:H100"/>
+    <mergeCell ref="F91:H91"/>
+    <mergeCell ref="F92:H92"/>
+    <mergeCell ref="F93:H93"/>
+    <mergeCell ref="F94:H94"/>
+    <mergeCell ref="F95:H95"/>
+    <mergeCell ref="F86:H86"/>
+    <mergeCell ref="F87:H87"/>
+    <mergeCell ref="F88:H88"/>
+    <mergeCell ref="F89:H89"/>
+    <mergeCell ref="F90:H90"/>
+    <mergeCell ref="F81:H81"/>
+    <mergeCell ref="F82:H82"/>
+    <mergeCell ref="F83:H83"/>
+    <mergeCell ref="F84:H84"/>
+    <mergeCell ref="F85:H85"/>
+    <mergeCell ref="F76:H76"/>
+    <mergeCell ref="F77:H77"/>
+    <mergeCell ref="F78:H78"/>
+    <mergeCell ref="F79:H79"/>
+    <mergeCell ref="F80:H80"/>
+    <mergeCell ref="F71:H71"/>
+    <mergeCell ref="F72:H72"/>
+    <mergeCell ref="F73:H73"/>
+    <mergeCell ref="F74:H74"/>
+    <mergeCell ref="F75:H75"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="F67:H67"/>
+    <mergeCell ref="F68:H68"/>
+    <mergeCell ref="F69:H69"/>
+    <mergeCell ref="F70:H70"/>
+    <mergeCell ref="F61:H61"/>
+    <mergeCell ref="F62:H62"/>
+    <mergeCell ref="F63:H63"/>
+    <mergeCell ref="F64:H64"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="F56:H56"/>
+    <mergeCell ref="F57:H57"/>
+    <mergeCell ref="F58:H58"/>
+    <mergeCell ref="F59:H59"/>
+    <mergeCell ref="F60:H60"/>
+    <mergeCell ref="F51:H51"/>
+    <mergeCell ref="F52:H52"/>
+    <mergeCell ref="F53:H53"/>
+    <mergeCell ref="F54:H54"/>
+    <mergeCell ref="F55:H55"/>
+    <mergeCell ref="F46:H46"/>
+    <mergeCell ref="F47:H47"/>
+    <mergeCell ref="F48:H48"/>
+    <mergeCell ref="F49:H49"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="F45:H45"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F15:H15"/>
     <mergeCell ref="F6:H6"/>
     <mergeCell ref="F7:H7"/>
     <mergeCell ref="F8:H8"/>
@@ -3532,196 +3725,6 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="C2:F2"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="F39:H39"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="F46:H46"/>
-    <mergeCell ref="F47:H47"/>
-    <mergeCell ref="F48:H48"/>
-    <mergeCell ref="F49:H49"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="F45:H45"/>
-    <mergeCell ref="F56:H56"/>
-    <mergeCell ref="F57:H57"/>
-    <mergeCell ref="F58:H58"/>
-    <mergeCell ref="F59:H59"/>
-    <mergeCell ref="F60:H60"/>
-    <mergeCell ref="F51:H51"/>
-    <mergeCell ref="F52:H52"/>
-    <mergeCell ref="F53:H53"/>
-    <mergeCell ref="F54:H54"/>
-    <mergeCell ref="F55:H55"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="F67:H67"/>
-    <mergeCell ref="F68:H68"/>
-    <mergeCell ref="F69:H69"/>
-    <mergeCell ref="F70:H70"/>
-    <mergeCell ref="F61:H61"/>
-    <mergeCell ref="F62:H62"/>
-    <mergeCell ref="F63:H63"/>
-    <mergeCell ref="F64:H64"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="F76:H76"/>
-    <mergeCell ref="F77:H77"/>
-    <mergeCell ref="F78:H78"/>
-    <mergeCell ref="F79:H79"/>
-    <mergeCell ref="F80:H80"/>
-    <mergeCell ref="F71:H71"/>
-    <mergeCell ref="F72:H72"/>
-    <mergeCell ref="F73:H73"/>
-    <mergeCell ref="F74:H74"/>
-    <mergeCell ref="F75:H75"/>
-    <mergeCell ref="F86:H86"/>
-    <mergeCell ref="F87:H87"/>
-    <mergeCell ref="F88:H88"/>
-    <mergeCell ref="F89:H89"/>
-    <mergeCell ref="F90:H90"/>
-    <mergeCell ref="F81:H81"/>
-    <mergeCell ref="F82:H82"/>
-    <mergeCell ref="F83:H83"/>
-    <mergeCell ref="F84:H84"/>
-    <mergeCell ref="F85:H85"/>
-    <mergeCell ref="F96:H96"/>
-    <mergeCell ref="F97:H97"/>
-    <mergeCell ref="F98:H98"/>
-    <mergeCell ref="F99:H99"/>
-    <mergeCell ref="F100:H100"/>
-    <mergeCell ref="F91:H91"/>
-    <mergeCell ref="F92:H92"/>
-    <mergeCell ref="F93:H93"/>
-    <mergeCell ref="F94:H94"/>
-    <mergeCell ref="F95:H95"/>
-    <mergeCell ref="F106:H106"/>
-    <mergeCell ref="F107:H107"/>
-    <mergeCell ref="F108:H108"/>
-    <mergeCell ref="F109:H109"/>
-    <mergeCell ref="F110:H110"/>
-    <mergeCell ref="F101:H101"/>
-    <mergeCell ref="F102:H102"/>
-    <mergeCell ref="F103:H103"/>
-    <mergeCell ref="F104:H104"/>
-    <mergeCell ref="F105:H105"/>
-    <mergeCell ref="F116:H116"/>
-    <mergeCell ref="F117:H117"/>
-    <mergeCell ref="F118:H118"/>
-    <mergeCell ref="F119:H119"/>
-    <mergeCell ref="F120:H120"/>
-    <mergeCell ref="F111:H111"/>
-    <mergeCell ref="F112:H112"/>
-    <mergeCell ref="F113:H113"/>
-    <mergeCell ref="F114:H114"/>
-    <mergeCell ref="F115:H115"/>
-    <mergeCell ref="F126:H126"/>
-    <mergeCell ref="F127:H127"/>
-    <mergeCell ref="F128:H128"/>
-    <mergeCell ref="F129:H129"/>
-    <mergeCell ref="F130:H130"/>
-    <mergeCell ref="F121:H121"/>
-    <mergeCell ref="F122:H122"/>
-    <mergeCell ref="F123:H123"/>
-    <mergeCell ref="F124:H124"/>
-    <mergeCell ref="F125:H125"/>
-    <mergeCell ref="F136:H136"/>
-    <mergeCell ref="F137:H137"/>
-    <mergeCell ref="F138:H138"/>
-    <mergeCell ref="F139:H139"/>
-    <mergeCell ref="F140:H140"/>
-    <mergeCell ref="F131:H131"/>
-    <mergeCell ref="F132:H132"/>
-    <mergeCell ref="F133:H133"/>
-    <mergeCell ref="F134:H134"/>
-    <mergeCell ref="F135:H135"/>
-    <mergeCell ref="F146:H146"/>
-    <mergeCell ref="F147:H147"/>
-    <mergeCell ref="F148:H148"/>
-    <mergeCell ref="F149:H149"/>
-    <mergeCell ref="F150:H150"/>
-    <mergeCell ref="F141:H141"/>
-    <mergeCell ref="F142:H142"/>
-    <mergeCell ref="F143:H143"/>
-    <mergeCell ref="F144:H144"/>
-    <mergeCell ref="F145:H145"/>
-    <mergeCell ref="F156:H156"/>
-    <mergeCell ref="F157:H157"/>
-    <mergeCell ref="F158:H158"/>
-    <mergeCell ref="F159:H159"/>
-    <mergeCell ref="F160:H160"/>
-    <mergeCell ref="F151:H151"/>
-    <mergeCell ref="F152:H152"/>
-    <mergeCell ref="F153:H153"/>
-    <mergeCell ref="F154:H154"/>
-    <mergeCell ref="F155:H155"/>
-    <mergeCell ref="F166:H166"/>
-    <mergeCell ref="F167:H167"/>
-    <mergeCell ref="F168:H168"/>
-    <mergeCell ref="F169:H169"/>
-    <mergeCell ref="F170:H170"/>
-    <mergeCell ref="F161:H161"/>
-    <mergeCell ref="F162:H162"/>
-    <mergeCell ref="F163:H163"/>
-    <mergeCell ref="F164:H164"/>
-    <mergeCell ref="F165:H165"/>
-    <mergeCell ref="F176:H176"/>
-    <mergeCell ref="F177:H177"/>
-    <mergeCell ref="F178:H178"/>
-    <mergeCell ref="F179:H179"/>
-    <mergeCell ref="F180:H180"/>
-    <mergeCell ref="F171:H171"/>
-    <mergeCell ref="F172:H172"/>
-    <mergeCell ref="F173:H173"/>
-    <mergeCell ref="F174:H174"/>
-    <mergeCell ref="F175:H175"/>
-    <mergeCell ref="F186:H186"/>
-    <mergeCell ref="F187:H187"/>
-    <mergeCell ref="F188:H188"/>
-    <mergeCell ref="F189:H189"/>
-    <mergeCell ref="F190:H190"/>
-    <mergeCell ref="F181:H181"/>
-    <mergeCell ref="F182:H182"/>
-    <mergeCell ref="F183:H183"/>
-    <mergeCell ref="F184:H184"/>
-    <mergeCell ref="F185:H185"/>
-    <mergeCell ref="F196:H196"/>
-    <mergeCell ref="F197:H197"/>
-    <mergeCell ref="F198:H198"/>
-    <mergeCell ref="F199:H199"/>
-    <mergeCell ref="F200:H200"/>
-    <mergeCell ref="F191:H191"/>
-    <mergeCell ref="F192:H192"/>
-    <mergeCell ref="F193:H193"/>
-    <mergeCell ref="F194:H194"/>
-    <mergeCell ref="F195:H195"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.47222222222222221" right="0.56944444444444442" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3739,7 +3742,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B7" sqref="B7:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="36" customHeight="1" zeroHeight="1" x14ac:dyDescent="0"/>
@@ -3818,8 +3821,8 @@
       <c r="A7" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="75">
-        <v>5</v>
+      <c r="B7" s="75" t="s">
+        <v>55</v>
       </c>
       <c r="C7" s="76"/>
       <c r="D7" s="76"/>
@@ -4046,21 +4049,21 @@
     <row r="20" spans="1:7" ht="36" hidden="1" customHeight="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="B5:G5"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="A14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B18:G18"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>